<commit_message>
updated timeline to use google drive links
</commit_message>
<xml_diff>
--- a/_data/timeline.xlsx
+++ b/_data/timeline.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osazeshears/Documents/Personal Projects/oshears.github.io/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1694F07-6ADC-8D45-93A4-BDB58C6E9F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B3D2439A-D401-4C49-846E-74D834963469}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21060" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timeline" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">timeline!$A$1:$D$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">timeline!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Cascade Falls</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Mango Comes Home!</t>
   </si>
   <si>
-    <t>Match has an Accident    :(</t>
-  </si>
-  <si>
     <t>Matcha and Mango Hanging Out</t>
   </si>
   <si>
@@ -82,90 +79,183 @@
     <t>Yappy Hour!</t>
   </si>
   <si>
-    <t>cascade_falls.jpg</t>
-  </si>
-  <si>
-    <t>first_semester_done.jpg</t>
-  </si>
-  <si>
-    <t>gia_grill_master.jpg</t>
-  </si>
-  <si>
-    <t>gia_matcha_christmas.jpg</t>
-  </si>
-  <si>
-    <t>gia_matcha_seneca_rocks.jpg</t>
-  </si>
-  <si>
-    <t>gia_osaze_matcha_vt.jpg</t>
-  </si>
-  <si>
-    <t>mango_comes_home.jpg</t>
-  </si>
-  <si>
-    <t>matcha_accident.jpg</t>
-  </si>
-  <si>
-    <t>matcha_and_mango_hang.jpg</t>
-  </si>
-  <si>
-    <t>matcha_banana.jpg</t>
-  </si>
-  <si>
-    <t>matcha_kayak_new_river.jpg</t>
-  </si>
-  <si>
-    <t>matcha_senca_rocks.jpg</t>
-  </si>
-  <si>
-    <t>matcha_spay.jpg</t>
-  </si>
-  <si>
-    <t>osaze_birthday_surprise.jpg</t>
-  </si>
-  <si>
-    <t>osaze_dad_zion.jpg</t>
-  </si>
-  <si>
-    <t>osaze_matcha_spruce_knob.jpg</t>
-  </si>
-  <si>
-    <t>osaze_start_gradschool.jpg</t>
-  </si>
-  <si>
-    <t>thanksgiving_roadside_overlook.jpg</t>
-  </si>
-  <si>
-    <t>yappy_hour.jpg</t>
-  </si>
-  <si>
     <t>Feels good to be free (for now...)!</t>
   </si>
   <si>
     <t>Blacksburg turned out to be a beautiful area, with a lack of good food options.</t>
   </si>
   <si>
-    <t>We visited the highest point in West Virginia!</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/ZPH9lpAa_eH6AOeskOXEQQ2KK67GeeFLI52WBFKxld6aFBEFGjRzEpi7nioDossGaEwCwGzptmTFS5sNO9hGTnOiPwuiSBeLWGCr0X01LwAmWeKuI5UoH92scagCx8rZhDjJjXK67R_32S46T9vtqsgumpEoyc0U57bpXoS3rXdjL6Oe0UrgoLKdCoiakwR7lQRGTVi1tpKt7ft8YPXDf-6SOmoIKecJnhs2BIzmMBFeAXr-lSRDj_nzfRSjzFy6XccVTei5PvGXuprjHTi-xdIX12lMJTYIuMcobbkuVQrMPYFgyTPckyfkhG_CRZlwQerE29hLsVuLK5AO6DpQDNPeQEjNi2VpN4DRN5bWQpjmgfHOAwKktXEvuWGGA-uz-t57zstXUoeAMDE3kswLJG2NRfhPQbDo-e23n3-l2SpY5fTNnUqqWV5frZzBzuE8pvD08yUy6MP3yLLD663x8e3WpAMMhcbE2dMKCc4TEuvI5Qbc1VmDjvSD_6XMLVbsmbkPG5okBg_l5ShypMkJ1x5ORX8XNbwDHu8m-xcytK2LxVqw1tz0lf8hkEhI4AdTKGEWqyTftqYpuE-BUxq2kLO5Z65Fej9r0DBTEEG5NSsQ4hoNydSqsv-fCgmvg-ejL9ni2ZPfgd7ifaTpbjqOj1hHxaWxIjoWpl-NrE7iSQxzpJ38TabNiG-0V7KEKQ=w786-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/bH8Wz68buoxQBrfsIJ_21jYqca9FGr-ftMezbcJ0XaymOfd5ucTboHdS_v0bGdku5L7TqE-kNi8cHXjVqJ4afEy6nFWBVyi57UFRel0IzxTi3UeLvJbeXphQYjPLaEu5gFHgX_vTMkMlGINV2n9cOTBymwfOo8x04-QKKZvQ0XOj8bVIunPjXLminjQ4iBH5-OeEuXTU0vB1ulLPZvD_10FdXzvdX_MsC7F6BqBZZdRR-seIkLngJ9CxspJAAaykMz7WAoCcKhHfdL6qdwyMFgly6J3lg7wiQU7_xLVULNRElxujFRqBdUdHYoSBfM6sWv3sXiGxQTe3_OA595A83UfDu2mDWye8HnpIyIKxiIexjBIoMugavKCZPg3uYz-xYHd5-H6-qtBOmsZy2nN9qSdTlvZnmuVkAdljiM6EaoXPOQzu_T9Vs9qDhZzfn_O9xVY5gYBMJfDAwq5lMRrp9ossGxdqQjKbPbTKKHnqQFnuLIBomXrbs3P8LjIl5k2JZZqC76KJtvkd5f_Tod1y9tAsMZzyi_FAWQibg3ypU2cnxu0Vu0p5Y1KNgabQ16l9I8QtcHZvoKa2w1bjvFgS7rIF2rIjkWuj5ZfxUKOX2c_39jurcrepQmUw2mRUwu95iP86q5socnJDIUMopVHOU7ajhLsgmEAFr4seQuN60i7vaHs6-dc-nW4v3mNXTQ=w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>image_link</t>
+  </si>
+  <si>
+    <t>Match has an Accident :(</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/rV96WBBt_DyliBlVcmpX8jy1rnYCCFMD2IIBhItiZTi9HVX4hh-wCuLR2KQTEUXTAGflScDqVx_GAwlwBFXhcE7am47I1wlZsmZHaMsEIpOtzgwTTLXLNo6uuFwlLrxKCES4ZEj95qXPeVeafz286k_8hxjkQJb8WeWW4wHP2fFFipyB3QOvZqtWR2XXxm3IWkAES7T1c2gPSxxus2_z_w6w9Bm63m5eegErfRWjKF-i9pjvsbUEDaAQH6O4J5iLHluSNckFXDWzwgCvkPWNlGV2IggAN0t7RWPgPoDSzVgJVy4vAaCbao3Ods94oldJcwwEQmv5jgLsJhvvuLAc1rcN1ON4LPDD4yFuCGJkKLz_Ut0lIOmTKm8BWTZ6q-aTiejFs-3biEAqCEoEQcdVv03Mh2lqUlHJogwlfmzph3x5T29CWfOzG_PtXwYag7-xy8iuAFvjPK0ZqNJtNrEwNXX3t51q5G4s45cB-sr2YpMuWtqsLVVDM8MYk07CLb1Nm1rxpKSrbESFPZL1U6gyZf1pw3_sxLUcyWDLg-tHMvf-3FTLM6rhoNqNNS7pptCns3s138LKxHYHT9XcCevMEcUdTc6uR60xoXNrR1sWi1m0gabdh5tBp940staAVjEu9lgvKzCkgY6eXTP1kSkK7n_t8Ab8aWJ-120un1-YR-aZ8haHVZmr83aE6N1yrw=w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Matcha and Mango Sunbathing</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/AZT4UK7AowKsOJFC4C7NiGfm0t1rIkjnq984D1B-5uKq-9eCAMNFtaWyu2nPBKuIkK0gaKODY9NnSgZ-jshcScPvUMCGdkBwvahRt6nUcbmQluL7Fa-zpPoiS4SwWXlsMzC1tEKL_kZdrF1louqBcv_O0bfidEq5Fw2T7AfPIQXHXao9Ua6wS6y7mI-Tn1xcnJv6nOnuTkZ3fmGFw2gOB_K5JczCxRzUKKE_Cdmgop0-_ewGhS7kI-hzgNrMjrgTLm7jBEtbuNbY9owd6NL6giYugGo5zgIVsOBy42Hc3V__pdqPNq8Ho868U1HnT0AMDct04cLM7KvQ-yUYxtPAbaOxKpRZX9sfJtraxsa5Qotr_JbhsiEJYHnWLk0YidBYIzOOaxrNeLZUaIIxitBQdBA9cMYnic0mvgN2CKW5gdUDhxyLxYvO7SajhQ3gRV_pDr9DtaLdraSJemHxNigRDffRUOlf0q5q38aIRopkpGtV0LlRIY5IHH2ao37TE-uQVezLsAm0B1oiSzoXcqw5k6XcTJ261_ZbZNFDzgOl1BYmlAZ7dcfT4gEf2pkvIfXF-LBKothWTQkXv0Ws3t0H9SGWGrz7TAek7tCrsx5rDj229EDjebpcVEu2yi8G9hOomx0tXrTrK1tfWMmNVAC0PttML7J9AI_Veny0Eqe-HHuAmejwbse_ia-NV44kEw=w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/HfxlqSoV3S_kU5rhGLN0rTBFlRJOcDI7pfakrVRWMulcdENytSELm8QLc9y3lPlU6HBlLWe6EXp1O8EjZDBkYwG7L1FnurUIZQMBwK2Z2B3-aiaF6VS71v_7cRvs-whe10zMHSDrfAS-rJEIU3UGFqmVUJwgzGaXmWoiWajuilHgFRAgAHCrl9ZuqMMSiol3xedsIBAAbWJKho06fhbJ0Gm8biN77r2M494ui_-l3X9S6EIsoa6i8r-54gxOQ24HHCyrTnhhJ9Zwyjg9JKEk8Sis5viP13bz8VxwtSx37-J9Ve0nUwH_bkJogEYABOOP8tPFdYxxk-NOP9zdkIE7hNEuS07PXdDrjVlnlwXIMbwbd8BlijzJIxiA7PdVG0lf5VXByC6kRa1B9mTYCwtNUxDq2KRzwPZg1J1BvHClbZ9T_uFRGjyT96Rx8EfeLltb5CTSPlEMDuma-cVKZ1Y1TEgitMCOQBBEREt1QAi-hxBsHF12DMJsfYK8JpfSVmBcV2lQwvliQv5NDwDVISYjg6ck_u5xZyu4qJTWrldLpXcFeB7zg0V24GC8FUiUVeiePDg5GByXegImwwuOfNDzxKuA0eSbY_IWW19UiW4t4_HdJ2X5FmOH5ngKv1GsMmZtgEbnaolJC4bhzThijT2teGO-nuNl8CJ05YDzoGiuZBIro4LSZmR0bnXsMJyDmQ=w786-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Mango Claims the Banana</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/T0PdM710-MP4Bc3rrNP5U9qW6v5ZBFP2i3P3bNQxNyh-xdahEmhRdY4eZk0sNxYFHJfqMc1qcn2NzPja8sAQkCKGzp9DXiEAoIFKlpP_EYXJJ0X-uQKUJh2-ejaAvQwVbh-32groCiyqIQ4HzWwALU4m-Y-qEtyoLHweZRsd7VfTaIgI-oGCn-LGV02OdDkoFL3wO6KIUJybTFIGbO2U-3X-QnNov5Km5QhaUnUTEtH6pSW60rzV5V5XByoSZJOPAeX3afUr2JAIEeXLrNoKDuqe8NCyNWHo6sCaKi2o_GYS89r_JdWHElVKxaPmGvLv-UPk3EQ77Lqz6TQBARoyr1XLKbTaU3_QfTQDFREHVAye7snWjL0CW9xiejBm8v1gykWRclhUeFQDyeUzf3MA0-M__Mng4G17iBW8OHRkP9Y-KYu0KffYqFomgQ7obsBAXd_hgZ0gM73fJ7xSNFA8ni2PEnjKYBrl5iwEzm7TAbiU1HfoUxjXwUUlIKN45F2ZtiTfb__ExE4gInl3CuzEgSmhG2WLbWLo3cggQeQZUHm02liettWKJJGmviT4S1IxxoM2lP26K6jaO_7ZWX4Ar2IZkPaUpOTQ3mlzqjvT32hB0fcJw4vzXVZAGulRyQmCkU-YlpBFCZdd5CuvMO13pcwrmYmvPrBPNfERHvyaZBDUTe4YY1XuiSYHQRk56Q=w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>We stopped by this overview off of I-64 on our way to get some Thanksgiving Dinner</t>
+  </si>
+  <si>
+    <t>Matcha and Mango's Banana</t>
+  </si>
+  <si>
+    <t>The two girls have decided to share the banana bed :)</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/hLgXLUZjTqWMRcJS-97K-uBUrQoxLPhdGjeMY9a3GPMs3BA6WEyF9aJIQf2xUeSsB3frB3vvljo-rsCjOrzO691xMFz8DsjiQ14DVJUmPkshyFplysu6FD9W4H3vQsMgrKUv0-eOxxNPrJ_bLBbnAqs-w7PEwToEjweoDUCk8gOzozG6ayTTgEP6DEZjEcHZYsEGX4Th-3AOvfhCxVqWF6dm3tELMptdklcWj3hsVWo2D67cywBSEVE43KEFeRFsfcCSC6HROQ-6RdE4dNq8VlSmAE-RZRGDz7Zvrt3PV6IJEkZgjULXkN12vC_BspVt_b0vLQ4gG1XioaggWMT95-VQ4K5Oy5cTTV_mrCkHtJNjssviKdb2myQEeHB_Kj1-ikXEA4fR2OBL8YabNrn42Svb0G2pe9H6v-lxU8zn0wNn4NLt_ntDtq0yEyHdK8oLCSmrwNwzpKYA4waU9Xe57r3RuPMgAU-qyQB-bVdnWwVQLixgdSTfhR9NwiwtoNtGkYCru-Oi2fdhfrNUAKcumyp4HxlNHizS9TTZZU6hgteslwFVpJcuWkf3js1R1cz6TtsoMGODy5vdK1OHFiHzC1ptg_ziqTqu3iggOIeG5YMkYDX2FHgQLJ8L0REvyVbEafetODxZlHtwuPr54HtqUcqgMmC0u4eQ1viCisqR0yxHPJ1Cg_-7dj56NBhD9g=w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/D5rynTmqfllmbK-Y1nOoRd1YBSnHdY8DIcyjdxVVT9ZBiETtqZx4hiPPIrH8iBpoXdgcb41pIQe47o2rlOK5-42FVju1JHuuiqCnm7UU-UqA6ipkyUuhTH8Z6bvS83qwNJ277Tmb4yIjhVIWSt8uMptbnhAY5CatxV3FMi-gjwW20R9y0XFBXeytMEdmjFFahJkT_jzK_-oY8JcI3xE-QERT7BdYWyoCJo8jwhxSpvaLPABu47tWiaSz1LA5t1dzc002QmM8-kUVX7GmqTU7WjvNdYW9QP1h_V4YpGQ_dufRwervT_gob0mjG0kswNFOxikfCOMOKqTwBE-DGLNnOc6Ak1hv73GRA_Ob7MxgG8S_nJYKkleBgyySqvY0My0vMeGYJCdBR2ELO20VSeX9DqTAgUt4Np6O-X_0B0kv59BO0u0yFf9BJdjK39XiDjuqdYvGiQJD56FqbR7YtO2EazAAuvCs_HcedaqP11GNtJbY-pT2pwcMgSRrXwVcMwXriOP6LlZDdZhKT3Z2VmV0Uti10A4qXloPYEp9Pk5ZQd_qNkCh4dSyL81ekLtQ1HxhtdA8LBeQ55fex9vtbl7oSAlvtBcVkWQi_XVkGPX-t-qLwJbfdW4qcqof5k1tRE8uUmROFxt3bHk2TYqdXGlIw3tyNcAMaQ1-WI2LZ5TzLpllGlpc5DDvX9xcn05Gvg=w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>She sure is the little hellion…</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/02EZAv9mO09FqxLVjQ3MTIDsZCPvcsAzN6_0P2pi240VNM5_4cOKYfL9wbEy-yPK9c6RDvuQ0iR2UN6MCQpkUge99AKZFACFjT7eUt3zFbyQPXODkTlCFJhyMD6DiLVxeScZoq9Mo5jwuu1PqrTl2dFq9SiAX40OH-U6XX6U-ivDwkukXvvBGYExoAH1vN5eN-OsLmYCatBiDbONgKDNfLUzjDDalVl1UCiQXZkpGFXkwaqgmiVsQ1NdyhXVo80BV6UnIRYBGYziQCtx2yVUi0LPdKSBWvAtN43QZAyaqPUvTDG0sMeSG-T_BPKoNj9auOR6oIpEDnzddfVziS89uy8NCRt9Zpou4hrXau6pKDRXHk9hcB6EnvP29WpHkONFoUvQdIHLiNjsYofPe4LRDNoe6-VUoGYIH0ENKdQ9L0VOgH0Cpl4v-WKIihHniJfmL754QxfEzruwttGLaV49b3t_lB9lVCniHjo9fJTa9M03ziVnTDLtK6bI5Kf27XzPI8HQgNEAGqveAZpyivIIF2du-hlpj0ethUucGfv6PXQbiBLT95Vlx-lB5AWXlBmG6hBGFA8ZjM78UoqLLkAGKXULio93bY2qCfl9KiWu4kGpil_ESTNO23AeSUcimVBK_Z7NuZx1nxtzQiur_gS5hoY0mZAtBL8mWIZMX1sxDTH0PWA-4p5B4Rz-i2ahSg=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>We were super excited to welcome Mango Ha-Shears into our family.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/CCyMxiG41ZDTWozj0TM1X15lD1EV3J9whovku7kl0Eh7eh_oUAzVdNWO-Ee_Xent0wMnqOcunOSQjH2HsxkY_gIb1E74vMm2XkmNg7gnc7CP2Pf3w9RefK70asgAWJPRxCvC1g13Ijtv0j9OVSUyyv5DpRczyPhkCk-nxdIwvxxt9vKGhtMG3jIlRYtPCa54j1TZjAoQellmr56udyLKsTj4UOKLr-FYiakd7w8GrPv0AA4Q9_Bj7dsO364-fSyo4tphBDoq7IyhP8kw-uXbSI63haiMEakFNim_WmNhb6MgYSwzPIATKGhvbY5GHd1mnocoLqGzYHWGmZzoqVZbziwPkdZUeKQ0TXVxMzFwJ-K2I6abqHnljAHFJqhfwY3dGXEO-2uvnf4eoG5g6Bfgvpu_z1r-tNNFrASr29Xizs4fucR-e0zUGU9ZhliFeTb7trKuzq_nuBYPTY692P--jzab0xIVxfRUdAkcw1qo56wkTyAYRMyXNZh4NVgMuWonlYxKHLDmduZHIenu8OOBopl4KkH7eKXnocoaCer4wzVVHmvkTjlCblSV5ucukj45iEFYzFOqKc-wSBCXIn2_fnMC2dqspH7SS8FwisDsa8QS788h2WIyXBDIsKBU9G4l5UTx4bRw4kR4k7eUMLRjiGvIX9JdYRpRr6dg96PjfWITJytnVFZvqzC2ZQeS6g=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/4EZ_5Us3G0pVtWXIKh_3Rln0-jZOMQzEgk8GfxsavVQ-_2x-WW4KUgsav_ufa63GS2c2Sg8svigNj5bGPwGx3GaICu5n7nvO-4weqNbHMPIsDhJ1NDcJA7csy9x8ZHs8HZcb6bBsye1tEDLuOSS4ICFW0NRIGbKumZVUm4g7-G1W_OZk2w9YKWjEewT1QI_WcUAu_Ov_KLBHyAPK8PSMzFGs3-eGkRIg0zM1olBFs6cKewJsZhlR2gLk-FVRe8MZ-KtMqmLT34jeQM44iLmdwfIqDk6vJ6vtJN7jFJ9OkHbxOKLmcxqzsyKOes0LpVUGccNMGJ5UnJPL7qlC7pseZ5OQaR816So83PDhHQOMh_j_eIE6b_8mkU6sYssjf78jI6rFaCf03a_aJ6mqMKMiUwLqAcC5Zzmv-VQgHtkAb_G4XB3BrQrw4Perti6RjHtPywT9G4zIX9XIC3Zb2hCCA4F0JFLAJcvpzpMpNVWB0YlKktWUXC62hgrZhsUtmTLMsf2PrLEpaXuSi0M5-2uvHFQTPF_wcIEHP_wrjEYIiYDR4zlWVEOc155xdTh_bilTKxKKQ7QEKVv8YsETb5iP3Y7sNcN8fvxTALNze9ptLHz0yQKkAz8HlJgEN-6y5QwNnIRpRGzU0lkruqTL5sFEG-qjXU0FU4-ejXX4twN67sXbWUOEAJI0Z2YaySVjNA=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/SO7A4_KzJ8LRNNjNjUkRmUDYzh4QIdChD0wPMfwHTg0lAeRSf4nl_4dkkpxMFqH18ZEh2DoPSEWNcgPWuE-zbv5blQG62AMQDPNQEcESQx30d8htD543zLt1wkqESFa5BnN8iB1WPjdePxT20Inx1Q4zFqNUXN5lnl_VYBf7ZqskeFPrdSAgcdULz46R_BE4LtxKQel6C6nOdBs87vfbahcrdwMUSkvWg755RWTnfynTGr0pz2RM_CUVLu0F-144iqO1v5FMkVS-F36RZuvA9jZyQW9AdKarxj8Me2cbs-VpKqpVKB1Gh_nUvQvnMfxvM11bDbHC4oktEWSYHMVTMovObGru7-d3d4QyY9a3bZYD9T7_VT46lXuMvWbJBvfQmYB2o-YJIR05XJI6deDbMPJEgClSJN-MYP7iDZynhjVzl655Na-rrMQnpSy50fbz57djMFqZCBBO1y00YF52eOfPwMhMfaR6k7Mh8Iiyb54cLS9PWuPfMsZOv475t-Sgivb1ymARf0a3thjVvqqqpix-8w8p0bqgPQhvwFg1nUm_PNHMU7Jpnv3P1jMuYrOjE3xSvlTy8bAMciAXgBQnSB_qiDPUqiu0emMiW2rFIzCB5s9keq3ppV_X4vWwlMdKuDm-jfPF8V8M-Jcr3Jft4w-dcljuwK6PAMDdHsjQ2mEeYrDcQaPapW0qiOACxg=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/e5LfhPK3dX3G0A64dS8UCCKJyNEnrt5egaCDKEIXlgtTTz8OXAkX7Is9zsrgXNpvrSrVc3yybXkVFVYeaU3LlKIHDjKrDhX1ObvTeDgxUisT9OWrj0CLjl0did4O4mR7-aG70Bx0clfsP7_KE2umqn8iCTljQqBfXYUPE9nH3S7K7aGR5n16GeIXyOTJIgYoKbRlFG0tA0nFCwTYlKJkEx3u3ovCo2chWbsRRrpj122zP7nD1gS0Y-dcALJBVhEZIexbOGBkP0G6FoNzczbUwaAg39nCA5Hp_VowAuQNFS_2pdoWUAkVd2EBC7UefmfrxZFngVPv5X8d-9N-bWpS1T6s2nS4KRoyVLMoNQ1i8it4cIkeb72DxCV-NboSvav9BAHVr0uSrMuz_krFzeVSH5FbLehyKsSJuCVsNOWkMcTgWHFVxLj9HC6iT2iA62y1ujvB_SDD8tr-hNLk2gdjIpCWvQYvcF7bSGpwJlT_yTqItjtrefeybeypa-Z_fvLgxdLXBpVFkA1gG_lcAV2tJ9fh-oCHYllH3gu_O4qXcMPtSrJ-BnGLnauNgNtU-85xoEFT4pkmBvYB6hhJbZ6o7QKlGZHvbMkPeu8yRO6iA0BQKLrERBfftYDw1gnGcrI4JOHCwu-n-0RAXgSRaxvo-JC3-wmOcwhvA-pTitv3DYIGL4bIRccCQpCrKOjzCg=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/XtJvfCU10XCHprNUOAKaj_qO1pgLXB5vRC98qnyKxK9xu3dIwL1c8np9uzA9FXAy_-ZagoZ4NhrSkalYzhBtf4kbnD6POT_dz9YvSqJmum7O2v3iuJSVF4WUBeRtpoW09P6IrF1gs7HKAQuQ0iNsuoKEZmDlgGzjrhi1YKrSWpEZj8D0q6v1Evkfx-7CX7kzuDCxETjmgjHwy430HNdRzmkDgJu9cQiE6zhzLeoTE7QWm0W6t9gdSB3eijfaXuUJKnkoppr2LG_zZYyRDDJA_GIlfADcWAS7alUPbxWqXeYP2Kr-X8sxGCqpyNxvvgEhfchAECyVoT3a81iXGf5yuha05VxdA89A6wmxZN4fNO4N1nUVtHUElbj5c_-6ahOhfwZDNDyoSs4uDrIEsDnGS-x1RNgE-oAjIhbDNXdImQJXnZ217cXlwSIgYjO1ajpZjooR_CLmdAqWSKALVsrGUz81ni0QDwgYuMTvwP9dOBoGbm4gJdwyR_PYOxAWAo8f2znDzAx9tjw_TxUCL_iQTPVLVhLSsmtnOQWTsUYiILIkQAjHRSRVGQTX-Ttpk-o9A_Agz5l0CPG_vdrk2Q7vgYmIn9EAENII15WLUGYyTyhvCog_P8aPL0ewAxPbZTd6L6TPzL9pVQ-ldEdBc1j12Gk6wJLLJgZvduT3ZS5zTVDyFpV9dCT89ZLJghbROw=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Our old friend Jason Pham comes down to visit us in Blacksburg and hike at Cascade Falls!</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/_kHh7qGlYsz-hxYnmoIh_yR-ggt0uWX5s4u_JcFTqFux1DzYnBTvsU5Qyw11MvbxudeeBGYOwfATrawOtVeQ-hphhDYu92JWIOjmbs63AbUTRRs3sfeGqkNQ5Df2FCAmeQWujagmQpf4Y5c2gAxU_b0w2ocWxvY82dNL2AJ-r0p6KJmkTFTnICy2s5rLIckHV4qRBvwqXrEYp9V-PjymKxFj9hTM-ruVE_-WnX_eCkMgj2sXfHy3kvrwyOvOXnsz8gy0SW6xwK6TpFVAZbgxYaxAvpq2gpAb0CAw9_t9Ve-vAZKaO2_I95b1FpvfctgX1NVCcLnPyltz8rdWPN48F03xFV4YvOMIeenZPUuemzHAcDi4UsfViBmBQMzuwVVQx7Q1pmSDfCyNlBtn4SDQQLVDlP9Rvv2qisQ3A-g8OSEO8qObaf-Zzg_dFzFWaBAj7Xy6fDGpcRWNpSYcVcIZwBw6iuEnlSaP1k0OpimUDzZiZ4RNDJwwlj1kRIYgXXXZZIctXctVQ_NX-TpRoByjGXeiiC8TuzQ4crijnJVV5Js2YDba2gU-HwaVn9tWXO19sQKB6SdFTiX-Jl3a3j38cYon_49OgBbOOdIWFKdfG9dnKyZHbjxt7SuHcagCOHs6X19U6ReNk7f-nbmJx7eZ6i5XtgLo4Q-TOa_f7RkHaU7aDqEQ7XI-8o61ZvqMTA=w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Our first time kayaking on the New River!</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/eFHQtqqkke4lyV_ftYOz4QQKETn9qwHXnMEOoKRE4OAUoj7tjZEgGpvMvzcGtYEnvxoX5S95R3cdksqi8RF_wO3msUkcRueOBAUr2U6ZYDzzOnEGanc-OLCeWtu5JuA5bXip6KW9T4XD0XjFhO_uBcUBnY7P2UQMYjDbSLfJ5m36fuSGCxKwfRISEE27j8EvA9VWAU39Nx1nXl4jc-cAdVKDwU4okBX9xp91N9NTNmCbucbYnyLNK5NoWfqo5ShsgmqsHSykMD6LcP7McRlm35kdgHRkYlUx9dqopoLYCVMiJ3rlXzY73eARFHUQ4I88fWNRmbgMyX-sXzuIRzDBqrKu7O08uhIZR5kHc5qKOYZJASpNNn1NgwEAEEKQycTUaoSJ4gAtNPzZiGEims09-ENT40-oWr9UPMEaek34BPlaEzmKplxZuFlfFVessyE-oBehaGCDR7LTqQgVYgDwvJ-Of8QuwShPlOkXMcrXdZjZNLdaXwjavS9NsiFmXxbNDDKK68SOW9qTSLLG8YTBSjkW3_TmwvQZ44ITnONLNOoVNtP-2wZQYv-Hw8vSPLFo3E7rIydRx1BKXywyDy0bxHV47v9mNzEBy9ibY73cAifb_Piy5gS0kB6zWtf9P9y4u6Bbg1gBEfn9ozEkUcSytBeMK4y_k8lZBnA2QTebpf4aJW_WwxSAbxKSpoCWyw=w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Matcha looks just as happy as I was.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/7DdwlbCpy6AMnGUH9KYH-IX5ifrNT9q_yOlqFc1hj4ti4CrxB3OQ91xzsL8aOi-FU6VG8FvqFNPgbI3wTq96mXC1rEMtCAheTcNQ3ofcs2Jo3PdypufUhcLpcnWH_sY5g7avqZylRYcuQBjSuUI_-BeHe1r3fZdFBDQXlr7y45rWGn52RDqKmQR6Cj-ZkHWTHRPjtHSolmsCT_zEnjBEnvpWTzJM_UjczC5uHQZwy1u9M64xHrgc67kdOfgKgy4IjFoNNyh1iI4KVaSqfa-WXRnMzeBBXxzU60U2MMnb3ryOvsHb50y1VGAbokH7y7fwuJPjnncW7iPT8HBVX59j1LsvsRQY-QbjLLF4THORp71hVJnMEi9u2irAbNbLHQ-yYnmDr4WraL_nWOuXT42BLCyTkrcfzOUCXaxQgS7sTk8bxA-HzQVo3xmFMFo4eSpRDjJhRS4JeylcRkK84_r4Cd3tLfay0v6OSp4hQGVxc02an234ghaY7hn0XR0Hhx0zcUzor9rrXH3ZJSQ7dpMkXNF8YiEk_ftYfVz9UMntUjk0ewkxgCHatzKwZNXzt0HbHstN4Jpy20MIE29avVbj68ET5OZLpmvokEgM2QTdPBQyKJAVu3_KGZjbQn4-M5hHxxrxkcVuJQSDwcTgx9VcEsNiNTQEJqp2f_Hs0duhisKVJBZs8w15DRSROf7wtA=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Our apartment complex hosted a Yappy Hour!</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/yFm9h1jOzp7kctZ9Ev0lx50b0RNWRBmVSMrLZ4XGcZ4akMHyEDjfjGVvYYgydMcdFH-UMgJMfTrLzO-yGQUFAJ9l-68QlqAlwl2QVwxP-odQQjJcOU62xTekgLt27KLD9apXCTBUa6bvD8lzmgaqcGmc_FIJc2Lg5kAVIo7OlsYCFxxGy5SSub2QKhiJ6hfKhgojPOjCeDQ38glfVmdnAr-Lg0FZVRWan-YtMWMD_fwuGBAAhZsWtpT5qUKrXHnWqNcDoSw07IzLuyA3LIOYyp8vbdqNHxD2dI0XQ_y3EGTxbvYqjU2O_vr5uDXaWb8VaPDeRRa8fiUJbVaa0tHSMzvbuyDnZ_CcH0543tiMtKXanr95n7DZRKo46Zwn3x15BKUH00CtxcsOpa5kumbVlqUA6wRSDn6cooivIojBrROWJtirWXBaSPdqXgSvs_qnftnnjT3da-rDf9KFPKalprdAmDYeROaOvFvMz7fLqA-XIDlg5m0eIMGwW_5cA1cXzYhF6xLH9pFl-LzM52rb3c9Pgsra9j0efFa5ikenzg6iRVjFCZH4Y3_CdOj6O2j7NvBZD8GMGlpr7L8Ry06bVMwpa4ur4gSYAcxrfpLcQpUOb3geAz2c2Yz7mB8VQEjd2GtTBCLa5JlV5wByFyQoefJi-6G2z-s1ctGZSV1O-5JQ7JokjoPYvufifk5IuQ=w1274-h588-no?authuser=0</t>
+  </si>
+  <si>
+    <t>He's a very proud father</t>
+  </si>
+  <si>
+    <t>Gia was pressed to cook her corn.</t>
+  </si>
+  <si>
+    <t>This was Matcha's halloween costume.</t>
+  </si>
+  <si>
+    <t>She swallowed a sewing needle, but came out of surgery ok!</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/0a6GkgdUgbDItBTH4LOzqpScoeBG6QRC767x9oo7r-JA-UxOFiMVId7eAZScnqL0yQ3KXnG_Ct29pc_imog92kaO1yrBHh1k5_XANU76GxQis6ng7UEtFopT0WIeTRmybJn7yTgpyV65m9-f8W6jf8uxZtHi4-4EyYbW2xpazdhjR0xjFKLT-y9smaIhMrqmY0fSdSE8J_537GyC0rMbqJvEfGpx0oVwyu-5YXpSNgKxJa8QYYI1lLizROzUubpG-Y_qyJcoAzJQwYkZ46T-cpZ68hOYBB_PDIlAMunFi5ekC2xIEkjJz00HuLd-2RlI-mtWZ9oJzLt66yJ4kcuh1kqM0uPPVXcSPohwntFwxBGtPJl1LD2L9cJveBQUh74-AaVMUSTHgpkt-XRkhD5iXTayz49qXQnIC9RlvTlr-WclffMrC3i5gf-OoQKt628bdjha-h99DfPQEN1JWMNUpEivNCk-gLOSTB8XZDhFPFmXqb74FJqj0kF9yF7PKv4PyL-g56e5UXQC3NQFkf2gYHAbjPLdtDdDYSpiM7Nr8YZXYDCIJnRmLhYpUUgG_5XHxTVSHhwQ0nQWcaAZiHUxvwe3T1gUyhRoj4CJAX-XMglpGtOlH_vwbJutRVyQFSEHv5b1T50w2z1dqQ32Kmc2etwc0xMzT1v6omi2_9ca_1Qc5YlYJIX7A1ybqiKEvg=w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>She came out of her spay procedure ok!</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/QsWCMC9C_fQrV3iQX_A0hAsHb13ox1-Xn5MjWvxPZTzqkVFuQbDRRRE2jXy2yEGJ_QrL8Z-A-oMP8qNX5A_sNtXLPGN_OD4zccgEj0QqSqruOUKgDXrUs7F33G9KzM2AFxR2zCV-Y6GuqBEN48XJ5ImeH8y90VqrONh6BP55-rY0CsLAOrq_-zk8McWIDtuS9FfYda-vxs2Hm-zCvalAqr4kp__fIhmgC06ytXJxPI0nJCkBypE9u0YwVEQ3CWtT26XZkHObqX-GHnuW9e4OpR9_yWH7xuxEevGpF2U5NtnqX8d5LQ_Ue7MAmxMw9QN4nEJ1yq3dFHNm1ddyQ-I71pHFU_Hs4WOyPUqjkHUTYQuW_a2CSM9z5bUut1ItxP08AxUsjpTlR5XI4qCSwAyanoksc33aoSW1aTT2YURvgDu2w5DFtZeJjW3Ph4vjdbu37aTIROq6ImnN7gW-nneD53LvPfFvl1ewz1kndxL2Re1qyFs69yZl9yn84AgDFDQW7ZQilL7k4_j0YH-3WqPm2rKgfLKJYVQLp4TcecSgSisSGiT3ALKDdJ0JfK6ozinOzMaITT6FEQhRpkNcuZOZBFocWa7YVlJskOdCB4lF-EqyhLx1tWtgR6jbv3Ti8StODiOkYX9BOdYdOuW6uFh63r8Lum1dj-va0l6oj82_SWhmu7yiAuYmhbYZvZRTKA=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Matcha enjoyed hiking halfway up Seneca Rocks</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/Too6SbI2tVRrZh7uJHzPTYNGbaWJQ1ucD-4rBrGwZVfazgvqSKQDK7Jw_aSCngk4wzWL02UQlPbYSLbpXL4t5rNqraRU9_oMi-lEu6l5Vxche8yKYL0lwDNRleISboIAI8Rr99H_EtUi5NzBW8fGcWn2JC950C6grcjH3_N7DF9oVWePZ3ZQgkI0IwK06nalestFbceDOC0uaTxwZjPmmBaWcb9XLd3mX94oEbPVxaE-mGf493Ez9Fs7yb-5crLd06MzZQjqTpITJi2-IY_73dzRkm2X8n3INbH1BvNrQg9-ExFcXYuzPh6VjGRSnuePFkEM8OEYfrAbOCV3K0wKbnKWr3QAbcIjBKW4VlPoclo_W9nYRAaRAc8nt4Wfl9Rics_MmpuG77NmTTYcS6CnD-v1UL_4EG0qJZgv0gA-HMbR1Lq0fGQKfYkrU3S3S0p09-7hoPZOXLo4pWdzkeHr7a5OijdB34NVGuEnaHaPX1nDKERQvffsl0uHkly9PSiTSTiX8b2_pbnQzuy6BO9fXBM5wNe_7feFd3R-XqxHdCoVHsMeQIA1NYWTQPZWuz56mWdXsdIpquLWhh3IM9JLZ8NjtoTgW4kHox9WvR7UVbbIsx5nqm1GtNV1HhXf14YsEetluUmo3RK5WDvmvRcpJCHV3HJgqTVX1H4g68twk3eZuqVLMTyKEP08a2-NHQ=w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/HTBpijAIiDbJ0Kg2ps6MCInpbDhQTPCq7adLmLILE7LSyql-BcusgNa0ZD_k-TEuS9Gz9vWrGLgz99J09OMZWwj8WL-KOxdEJ855cHZwiM6f8Z85A4VBxI2kR7S4uMncC94myUa1R0JwVt7a3HXMjAOTk4aCz-1DAOFQ16WUn6yFxHUq87dTJRwRvVlcKrbrIxQvKHIpg6nYAPUMDbJNedq7JeL3HrfZvCvmfchWhfO5tnMCew8pvMDWMKSZ9Vl89a7GU0K2gZUqZMaHgdj02t1FQllZmFXmJ6D56KeYaLlAVTaInNZ9nhpM1ae7nTlioBo2weNOvKQto3xD8v_MX1xL0WFV6LzdaKAbKo9pA8H3Ws-7MWFMhcYJ3FIorSBsKr9j4s9p8N471PPzl6GC3SfbT3kKoAsH3Vdg_d4UxEbufmVrh1_FNGaghOeX6uJiEXv6osrFUhgFAHXXJc4IkQNnz1olVTivzm1anCGLqfR3QLicy-0p5BfzCsikrGMbySbrQwYrZWWWGa8FQ3lAAVJLejhVmDOJaYvQg7zqLLEOmAQjcQQ1sj9GTDO38CG2gYUt6qJpR86EQbt0G_WeD_KbGtg1o7bP0s3k987lpRKR2hRUgDImv9D_o9De4AV1cq9pIAdtacY--T7L_JpSxE45P__zyndsUIgd2HaWZLMu6Yj_X40-thP2H2hiAg=w336-h252-no?authuser=0</t>
+  </si>
+  <si>
+    <t>Little Devil Stairs</t>
+  </si>
+  <si>
+    <t>We hiked up Little Devil Stairs at Shenandoah National Park</t>
+  </si>
+  <si>
+    <t>It's a part of their daily routine.</t>
+  </si>
+  <si>
+    <t>It was hers first.</t>
+  </si>
+  <si>
+    <t>Relaxing as usual.</t>
+  </si>
+  <si>
+    <t>Gia loves this picture.</t>
+  </si>
+  <si>
+    <t>Each sticky note is an individual food-related pickup line.</t>
+  </si>
+  <si>
+    <t>We visited the highest point in West Virginia! Afterwards we camped near Seneca Rocks. The trip ended with a visit to Luray Caverns.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/ICR-H3rjrXPJMUMRdoyeRxYwUmc-PE3Hg91KgPdqiDK5x3Hy-tz5IV7YhZo0Y7ygcADLr3mYDjCFRUFmlQqFDCA35KdXMm9c8oFMfeN4-4IdyRdlloXD83B4OtuJ5ua_OuZDFVeG289Y3u0LkK3f_eWntskeRrRVXLAxlCPhJbIBUoCaL7MSBs8TvigBshR8YeKoGnFdsARP495EboFfXjg9-ywqcq8LgXoaM6fdXOyAU0p3xGBEb9jLo99rOYrfYg0z_B--8M5B6_o-rHuOClZPVb0IhO5CK_1IGRlKDxx7lGMQqqkmRWcVPhlELXpSHf5dWs8BLmOAqqBVHqNzPXJtSKh_RCqy5-zxnl9rhwH-nYxnq5tazRKRm0vzAS3iOOvfDfgc6wkapYWgyOzMRjoKsyMGRKO_diDGpo043IyxJRoqdgDqklSXrxP1dmMXEKsYYfSOxZlPN3JRsjI_LrMMOdP4TukmR9hTZ31I3CMXM9Pg-nXMYP4D0bHWeyadl2zEZ34e7ru-1fYN9OFQ4uAWi8drZkGs28cNtBsDKMBY0BzfXFuzpTUdm_20Bx7xIY4PdovjDeOCPMykZ4ZPHao8ZDLmMQegmU8F-uCi-Mm_HKDk9Vq_fveHXzBrcHMDwh5SemYM6RdAKXjrN4bgZ3qnw9hQoFq2CT4aCm29o5F2xEuAnVs2zSKoGAz8Ow=w312-h234-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/PWeCFi4Ji8HJisVP0udLQLho2xy9GHDOY0wkLzb87f3GyWUsAwpEjdX5Woi6qihfPaOAfhragg0Tx2n10-nvpfIcE_iP3u-f05IxAwenUeopYK63pnWSGzv84TqkDAIPSR1Pag_v_ODcU4L4F-cMgDUuWMn8g4iUjwoUBqxWC3Db5Um9sU7u7x-_fUf31RX1NPXaEaCSL9ocl_P0g-QNM5D8fswCaLrTGws1z_okflMrfaFpWSn3y15oOdXXiJ9hvLwyI9VHtYxwly-Ti5B7kOVBW-lWnYcKnnnUiSn6D7PT6wXUtLwXxvwH3UPlPRLy4rqfUicHt6zz3mGhPwWVE-Yi1ojT0qqvnDC2REwoLhMKvl8Xw9bE3S_5n2I_la4HrS659K2ttiMB9HVn7kDH84tl3rqf3KwOxSgrpn5JhiS7hbew_BaEBVjyhGE2xQfpI8_emr3FLwlAwLQ7Fawn2K9FXn3VhwiJDjskOpBx6tHW5ZANzeynS5DKSjz7EBNhi_-4OwFXndgt14au2IvoBn6lZFnXoM-fbkVGpW4b_bLXLzOErr1brnfkO7ZPwVwci6y3kavFp1psqEtiGOt0nbvJgK9-yXTuQ8fLm1XSAHtjFltJPkiQR07aNeuzK-bG3NuGJCiYrD-lSTc1DSMOaV7Z2X7ujlRZ8RtHnsVafBEwq-FbymccEpuNZTYdPg=w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>We only made it halfway :)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -644,10 +734,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1002,257 +1093,374 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>44166</v>
+        <v>44180</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>44166</v>
+        <v>44180</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>44136</v>
+        <v>44179</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
-        <v>44136</v>
+        <v>44178</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
-        <v>44136</v>
+        <v>44168</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>44105</v>
+        <v>44161</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
-        <v>44075</v>
+        <v>44154</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>44075</v>
+        <v>44148</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>44075</v>
+        <v>44148</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
-        <v>44075</v>
+        <v>44134</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
-        <v>44044</v>
+        <v>44120</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1">
-        <v>44044</v>
+        <v>44101</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1">
-        <v>44044</v>
+        <v>44099</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1">
-        <v>44044</v>
+        <v>44087</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1">
-        <v>44013</v>
+        <v>44079</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>43983</v>
+        <v>44073</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>43983</v>
+        <v>44069</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1">
-        <v>43983</v>
+        <v>44057</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1">
-        <v>43983</v>
+        <v>44035</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44011</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44010</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44009</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44009</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43982</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D20">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">
-      <sortCondition descending="1" ref="B1:B20"/>
+  <autoFilter ref="A1:D1" xr:uid="{4928DC32-4694-004E-930F-1CCF4DE71108}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D25">
+      <sortCondition descending="1" ref="B1:B25"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
started updating photos to have permanent links
</commit_message>
<xml_diff>
--- a/_data/timeline.xlsx
+++ b/_data/timeline.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osazeshears/Documents/Personal Projects/oshears.github.io/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B3D2439A-D401-4C49-846E-74D834963469}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A376AB-4CF1-4445-AAA6-8D1D5A299592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21060" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16940" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timeline" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">timeline!$A$1:$D$1</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Cascade Falls</t>
   </si>
@@ -94,36 +95,18 @@
     <t>description</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/ZPH9lpAa_eH6AOeskOXEQQ2KK67GeeFLI52WBFKxld6aFBEFGjRzEpi7nioDossGaEwCwGzptmTFS5sNO9hGTnOiPwuiSBeLWGCr0X01LwAmWeKuI5UoH92scagCx8rZhDjJjXK67R_32S46T9vtqsgumpEoyc0U57bpXoS3rXdjL6Oe0UrgoLKdCoiakwR7lQRGTVi1tpKt7ft8YPXDf-6SOmoIKecJnhs2BIzmMBFeAXr-lSRDj_nzfRSjzFy6XccVTei5PvGXuprjHTi-xdIX12lMJTYIuMcobbkuVQrMPYFgyTPckyfkhG_CRZlwQerE29hLsVuLK5AO6DpQDNPeQEjNi2VpN4DRN5bWQpjmgfHOAwKktXEvuWGGA-uz-t57zstXUoeAMDE3kswLJG2NRfhPQbDo-e23n3-l2SpY5fTNnUqqWV5frZzBzuE8pvD08yUy6MP3yLLD663x8e3WpAMMhcbE2dMKCc4TEuvI5Qbc1VmDjvSD_6XMLVbsmbkPG5okBg_l5ShypMkJ1x5ORX8XNbwDHu8m-xcytK2LxVqw1tz0lf8hkEhI4AdTKGEWqyTftqYpuE-BUxq2kLO5Z65Fej9r0DBTEEG5NSsQ4hoNydSqsv-fCgmvg-ejL9ni2ZPfgd7ifaTpbjqOj1hHxaWxIjoWpl-NrE7iSQxzpJ38TabNiG-0V7KEKQ=w786-h1396-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/bH8Wz68buoxQBrfsIJ_21jYqca9FGr-ftMezbcJ0XaymOfd5ucTboHdS_v0bGdku5L7TqE-kNi8cHXjVqJ4afEy6nFWBVyi57UFRel0IzxTi3UeLvJbeXphQYjPLaEu5gFHgX_vTMkMlGINV2n9cOTBymwfOo8x04-QKKZvQ0XOj8bVIunPjXLminjQ4iBH5-OeEuXTU0vB1ulLPZvD_10FdXzvdX_MsC7F6BqBZZdRR-seIkLngJ9CxspJAAaykMz7WAoCcKhHfdL6qdwyMFgly6J3lg7wiQU7_xLVULNRElxujFRqBdUdHYoSBfM6sWv3sXiGxQTe3_OA595A83UfDu2mDWye8HnpIyIKxiIexjBIoMugavKCZPg3uYz-xYHd5-H6-qtBOmsZy2nN9qSdTlvZnmuVkAdljiM6EaoXPOQzu_T9Vs9qDhZzfn_O9xVY5gYBMJfDAwq5lMRrp9ossGxdqQjKbPbTKKHnqQFnuLIBomXrbs3P8LjIl5k2JZZqC76KJtvkd5f_Tod1y9tAsMZzyi_FAWQibg3ypU2cnxu0Vu0p5Y1KNgabQ16l9I8QtcHZvoKa2w1bjvFgS7rIF2rIjkWuj5ZfxUKOX2c_39jurcrepQmUw2mRUwu95iP86q5socnJDIUMopVHOU7ajhLsgmEAFr4seQuN60i7vaHs6-dc-nW4v3mNXTQ=w1048-h1396-no?authuser=0</t>
-  </si>
-  <si>
     <t>image_link</t>
   </si>
   <si>
     <t>Match has an Accident :(</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/rV96WBBt_DyliBlVcmpX8jy1rnYCCFMD2IIBhItiZTi9HVX4hh-wCuLR2KQTEUXTAGflScDqVx_GAwlwBFXhcE7am47I1wlZsmZHaMsEIpOtzgwTTLXLNo6uuFwlLrxKCES4ZEj95qXPeVeafz286k_8hxjkQJb8WeWW4wHP2fFFipyB3QOvZqtWR2XXxm3IWkAES7T1c2gPSxxus2_z_w6w9Bm63m5eegErfRWjKF-i9pjvsbUEDaAQH6O4J5iLHluSNckFXDWzwgCvkPWNlGV2IggAN0t7RWPgPoDSzVgJVy4vAaCbao3Ods94oldJcwwEQmv5jgLsJhvvuLAc1rcN1ON4LPDD4yFuCGJkKLz_Ut0lIOmTKm8BWTZ6q-aTiejFs-3biEAqCEoEQcdVv03Mh2lqUlHJogwlfmzph3x5T29CWfOzG_PtXwYag7-xy8iuAFvjPK0ZqNJtNrEwNXX3t51q5G4s45cB-sr2YpMuWtqsLVVDM8MYk07CLb1Nm1rxpKSrbESFPZL1U6gyZf1pw3_sxLUcyWDLg-tHMvf-3FTLM6rhoNqNNS7pptCns3s138LKxHYHT9XcCevMEcUdTc6uR60xoXNrR1sWi1m0gabdh5tBp940staAVjEu9lgvKzCkgY6eXTP1kSkK7n_t8Ab8aWJ-120un1-YR-aZ8haHVZmr83aE6N1yrw=w1274-h718-no?authuser=0</t>
-  </si>
-  <si>
     <t>Matcha and Mango Sunbathing</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/AZT4UK7AowKsOJFC4C7NiGfm0t1rIkjnq984D1B-5uKq-9eCAMNFtaWyu2nPBKuIkK0gaKODY9NnSgZ-jshcScPvUMCGdkBwvahRt6nUcbmQluL7Fa-zpPoiS4SwWXlsMzC1tEKL_kZdrF1louqBcv_O0bfidEq5Fw2T7AfPIQXHXao9Ua6wS6y7mI-Tn1xcnJv6nOnuTkZ3fmGFw2gOB_K5JczCxRzUKKE_Cdmgop0-_ewGhS7kI-hzgNrMjrgTLm7jBEtbuNbY9owd6NL6giYugGo5zgIVsOBy42Hc3V__pdqPNq8Ho868U1HnT0AMDct04cLM7KvQ-yUYxtPAbaOxKpRZX9sfJtraxsa5Qotr_JbhsiEJYHnWLk0YidBYIzOOaxrNeLZUaIIxitBQdBA9cMYnic0mvgN2CKW5gdUDhxyLxYvO7SajhQ3gRV_pDr9DtaLdraSJemHxNigRDffRUOlf0q5q38aIRopkpGtV0LlRIY5IHH2ao37TE-uQVezLsAm0B1oiSzoXcqw5k6XcTJ261_ZbZNFDzgOl1BYmlAZ7dcfT4gEf2pkvIfXF-LBKothWTQkXv0Ws3t0H9SGWGrz7TAek7tCrsx5rDj229EDjebpcVEu2yi8G9hOomx0tXrTrK1tfWMmNVAC0PttML7J9AI_Veny0Eqe-HHuAmejwbse_ia-NV44kEw=w1274-h718-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/HfxlqSoV3S_kU5rhGLN0rTBFlRJOcDI7pfakrVRWMulcdENytSELm8QLc9y3lPlU6HBlLWe6EXp1O8EjZDBkYwG7L1FnurUIZQMBwK2Z2B3-aiaF6VS71v_7cRvs-whe10zMHSDrfAS-rJEIU3UGFqmVUJwgzGaXmWoiWajuilHgFRAgAHCrl9ZuqMMSiol3xedsIBAAbWJKho06fhbJ0Gm8biN77r2M494ui_-l3X9S6EIsoa6i8r-54gxOQ24HHCyrTnhhJ9Zwyjg9JKEk8Sis5viP13bz8VxwtSx37-J9Ve0nUwH_bkJogEYABOOP8tPFdYxxk-NOP9zdkIE7hNEuS07PXdDrjVlnlwXIMbwbd8BlijzJIxiA7PdVG0lf5VXByC6kRa1B9mTYCwtNUxDq2KRzwPZg1J1BvHClbZ9T_uFRGjyT96Rx8EfeLltb5CTSPlEMDuma-cVKZ1Y1TEgitMCOQBBEREt1QAi-hxBsHF12DMJsfYK8JpfSVmBcV2lQwvliQv5NDwDVISYjg6ck_u5xZyu4qJTWrldLpXcFeB7zg0V24GC8FUiUVeiePDg5GByXegImwwuOfNDzxKuA0eSbY_IWW19UiW4t4_HdJ2X5FmOH5ngKv1GsMmZtgEbnaolJC4bhzThijT2teGO-nuNl8CJ05YDzoGiuZBIro4LSZmR0bnXsMJyDmQ=w786-h1396-no?authuser=0</t>
-  </si>
-  <si>
     <t>Mango Claims the Banana</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/T0PdM710-MP4Bc3rrNP5U9qW6v5ZBFP2i3P3bNQxNyh-xdahEmhRdY4eZk0sNxYFHJfqMc1qcn2NzPja8sAQkCKGzp9DXiEAoIFKlpP_EYXJJ0X-uQKUJh2-ejaAvQwVbh-32groCiyqIQ4HzWwALU4m-Y-qEtyoLHweZRsd7VfTaIgI-oGCn-LGV02OdDkoFL3wO6KIUJybTFIGbO2U-3X-QnNov5Km5QhaUnUTEtH6pSW60rzV5V5XByoSZJOPAeX3afUr2JAIEeXLrNoKDuqe8NCyNWHo6sCaKi2o_GYS89r_JdWHElVKxaPmGvLv-UPk3EQ77Lqz6TQBARoyr1XLKbTaU3_QfTQDFREHVAye7snWjL0CW9xiejBm8v1gykWRclhUeFQDyeUzf3MA0-M__Mng4G17iBW8OHRkP9Y-KYu0KffYqFomgQ7obsBAXd_hgZ0gM73fJ7xSNFA8ni2PEnjKYBrl5iwEzm7TAbiU1HfoUxjXwUUlIKN45F2ZtiTfb__ExE4gInl3CuzEgSmhG2WLbWLo3cggQeQZUHm02liettWKJJGmviT4S1IxxoM2lP26K6jaO_7ZWX4Ar2IZkPaUpOTQ3mlzqjvT32hB0fcJw4vzXVZAGulRyQmCkU-YlpBFCZdd5CuvMO13pcwrmYmvPrBPNfERHvyaZBDUTe4YY1XuiSYHQRk56Q=w1274-h718-no?authuser=0</t>
-  </si>
-  <si>
     <t>We stopped by this overview off of I-64 on our way to get some Thanksgiving Dinner</t>
   </si>
   <si>
@@ -133,60 +116,24 @@
     <t>The two girls have decided to share the banana bed :)</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/hLgXLUZjTqWMRcJS-97K-uBUrQoxLPhdGjeMY9a3GPMs3BA6WEyF9aJIQf2xUeSsB3frB3vvljo-rsCjOrzO691xMFz8DsjiQ14DVJUmPkshyFplysu6FD9W4H3vQsMgrKUv0-eOxxNPrJ_bLBbnAqs-w7PEwToEjweoDUCk8gOzozG6ayTTgEP6DEZjEcHZYsEGX4Th-3AOvfhCxVqWF6dm3tELMptdklcWj3hsVWo2D67cywBSEVE43KEFeRFsfcCSC6HROQ-6RdE4dNq8VlSmAE-RZRGDz7Zvrt3PV6IJEkZgjULXkN12vC_BspVt_b0vLQ4gG1XioaggWMT95-VQ4K5Oy5cTTV_mrCkHtJNjssviKdb2myQEeHB_Kj1-ikXEA4fR2OBL8YabNrn42Svb0G2pe9H6v-lxU8zn0wNn4NLt_ntDtq0yEyHdK8oLCSmrwNwzpKYA4waU9Xe57r3RuPMgAU-qyQB-bVdnWwVQLixgdSTfhR9NwiwtoNtGkYCru-Oi2fdhfrNUAKcumyp4HxlNHizS9TTZZU6hgteslwFVpJcuWkf3js1R1cz6TtsoMGODy5vdK1OHFiHzC1ptg_ziqTqu3iggOIeG5YMkYDX2FHgQLJ8L0REvyVbEafetODxZlHtwuPr54HtqUcqgMmC0u4eQ1viCisqR0yxHPJ1Cg_-7dj56NBhD9g=w1274-h718-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/D5rynTmqfllmbK-Y1nOoRd1YBSnHdY8DIcyjdxVVT9ZBiETtqZx4hiPPIrH8iBpoXdgcb41pIQe47o2rlOK5-42FVju1JHuuiqCnm7UU-UqA6ipkyUuhTH8Z6bvS83qwNJ277Tmb4yIjhVIWSt8uMptbnhAY5CatxV3FMi-gjwW20R9y0XFBXeytMEdmjFFahJkT_jzK_-oY8JcI3xE-QERT7BdYWyoCJo8jwhxSpvaLPABu47tWiaSz1LA5t1dzc002QmM8-kUVX7GmqTU7WjvNdYW9QP1h_V4YpGQ_dufRwervT_gob0mjG0kswNFOxikfCOMOKqTwBE-DGLNnOc6Ak1hv73GRA_Ob7MxgG8S_nJYKkleBgyySqvY0My0vMeGYJCdBR2ELO20VSeX9DqTAgUt4Np6O-X_0B0kv59BO0u0yFf9BJdjK39XiDjuqdYvGiQJD56FqbR7YtO2EazAAuvCs_HcedaqP11GNtJbY-pT2pwcMgSRrXwVcMwXriOP6LlZDdZhKT3Z2VmV0Uti10A4qXloPYEp9Pk5ZQd_qNkCh4dSyL81ekLtQ1HxhtdA8LBeQ55fex9vtbl7oSAlvtBcVkWQi_XVkGPX-t-qLwJbfdW4qcqof5k1tRE8uUmROFxt3bHk2TYqdXGlIw3tyNcAMaQ1-WI2LZ5TzLpllGlpc5DDvX9xcn05Gvg=w1274-h718-no?authuser=0</t>
-  </si>
-  <si>
     <t>She sure is the little hellion…</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/02EZAv9mO09FqxLVjQ3MTIDsZCPvcsAzN6_0P2pi240VNM5_4cOKYfL9wbEy-yPK9c6RDvuQ0iR2UN6MCQpkUge99AKZFACFjT7eUt3zFbyQPXODkTlCFJhyMD6DiLVxeScZoq9Mo5jwuu1PqrTl2dFq9SiAX40OH-U6XX6U-ivDwkukXvvBGYExoAH1vN5eN-OsLmYCatBiDbONgKDNfLUzjDDalVl1UCiQXZkpGFXkwaqgmiVsQ1NdyhXVo80BV6UnIRYBGYziQCtx2yVUi0LPdKSBWvAtN43QZAyaqPUvTDG0sMeSG-T_BPKoNj9auOR6oIpEDnzddfVziS89uy8NCRt9Zpou4hrXau6pKDRXHk9hcB6EnvP29WpHkONFoUvQdIHLiNjsYofPe4LRDNoe6-VUoGYIH0ENKdQ9L0VOgH0Cpl4v-WKIihHniJfmL754QxfEzruwttGLaV49b3t_lB9lVCniHjo9fJTa9M03ziVnTDLtK6bI5Kf27XzPI8HQgNEAGqveAZpyivIIF2du-hlpj0ethUucGfv6PXQbiBLT95Vlx-lB5AWXlBmG6hBGFA8ZjM78UoqLLkAGKXULio93bY2qCfl9KiWu4kGpil_ESTNO23AeSUcimVBK_Z7NuZx1nxtzQiur_gS5hoY0mZAtBL8mWIZMX1sxDTH0PWA-4p5B4Rz-i2ahSg=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
     <t>We were super excited to welcome Mango Ha-Shears into our family.</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/CCyMxiG41ZDTWozj0TM1X15lD1EV3J9whovku7kl0Eh7eh_oUAzVdNWO-Ee_Xent0wMnqOcunOSQjH2HsxkY_gIb1E74vMm2XkmNg7gnc7CP2Pf3w9RefK70asgAWJPRxCvC1g13Ijtv0j9OVSUyyv5DpRczyPhkCk-nxdIwvxxt9vKGhtMG3jIlRYtPCa54j1TZjAoQellmr56udyLKsTj4UOKLr-FYiakd7w8GrPv0AA4Q9_Bj7dsO364-fSyo4tphBDoq7IyhP8kw-uXbSI63haiMEakFNim_WmNhb6MgYSwzPIATKGhvbY5GHd1mnocoLqGzYHWGmZzoqVZbziwPkdZUeKQ0TXVxMzFwJ-K2I6abqHnljAHFJqhfwY3dGXEO-2uvnf4eoG5g6Bfgvpu_z1r-tNNFrASr29Xizs4fucR-e0zUGU9ZhliFeTb7trKuzq_nuBYPTY692P--jzab0xIVxfRUdAkcw1qo56wkTyAYRMyXNZh4NVgMuWonlYxKHLDmduZHIenu8OOBopl4KkH7eKXnocoaCer4wzVVHmvkTjlCblSV5ucukj45iEFYzFOqKc-wSBCXIn2_fnMC2dqspH7SS8FwisDsa8QS788h2WIyXBDIsKBU9G4l5UTx4bRw4kR4k7eUMLRjiGvIX9JdYRpRr6dg96PjfWITJytnVFZvqzC2ZQeS6g=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/4EZ_5Us3G0pVtWXIKh_3Rln0-jZOMQzEgk8GfxsavVQ-_2x-WW4KUgsav_ufa63GS2c2Sg8svigNj5bGPwGx3GaICu5n7nvO-4weqNbHMPIsDhJ1NDcJA7csy9x8ZHs8HZcb6bBsye1tEDLuOSS4ICFW0NRIGbKumZVUm4g7-G1W_OZk2w9YKWjEewT1QI_WcUAu_Ov_KLBHyAPK8PSMzFGs3-eGkRIg0zM1olBFs6cKewJsZhlR2gLk-FVRe8MZ-KtMqmLT34jeQM44iLmdwfIqDk6vJ6vtJN7jFJ9OkHbxOKLmcxqzsyKOes0LpVUGccNMGJ5UnJPL7qlC7pseZ5OQaR816So83PDhHQOMh_j_eIE6b_8mkU6sYssjf78jI6rFaCf03a_aJ6mqMKMiUwLqAcC5Zzmv-VQgHtkAb_G4XB3BrQrw4Perti6RjHtPywT9G4zIX9XIC3Zb2hCCA4F0JFLAJcvpzpMpNVWB0YlKktWUXC62hgrZhsUtmTLMsf2PrLEpaXuSi0M5-2uvHFQTPF_wcIEHP_wrjEYIiYDR4zlWVEOc155xdTh_bilTKxKKQ7QEKVv8YsETb5iP3Y7sNcN8fvxTALNze9ptLHz0yQKkAz8HlJgEN-6y5QwNnIRpRGzU0lkruqTL5sFEG-qjXU0FU4-ejXX4twN67sXbWUOEAJI0Z2YaySVjNA=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/SO7A4_KzJ8LRNNjNjUkRmUDYzh4QIdChD0wPMfwHTg0lAeRSf4nl_4dkkpxMFqH18ZEh2DoPSEWNcgPWuE-zbv5blQG62AMQDPNQEcESQx30d8htD543zLt1wkqESFa5BnN8iB1WPjdePxT20Inx1Q4zFqNUXN5lnl_VYBf7ZqskeFPrdSAgcdULz46R_BE4LtxKQel6C6nOdBs87vfbahcrdwMUSkvWg755RWTnfynTGr0pz2RM_CUVLu0F-144iqO1v5FMkVS-F36RZuvA9jZyQW9AdKarxj8Me2cbs-VpKqpVKB1Gh_nUvQvnMfxvM11bDbHC4oktEWSYHMVTMovObGru7-d3d4QyY9a3bZYD9T7_VT46lXuMvWbJBvfQmYB2o-YJIR05XJI6deDbMPJEgClSJN-MYP7iDZynhjVzl655Na-rrMQnpSy50fbz57djMFqZCBBO1y00YF52eOfPwMhMfaR6k7Mh8Iiyb54cLS9PWuPfMsZOv475t-Sgivb1ymARf0a3thjVvqqqpix-8w8p0bqgPQhvwFg1nUm_PNHMU7Jpnv3P1jMuYrOjE3xSvlTy8bAMciAXgBQnSB_qiDPUqiu0emMiW2rFIzCB5s9keq3ppV_X4vWwlMdKuDm-jfPF8V8M-Jcr3Jft4w-dcljuwK6PAMDdHsjQ2mEeYrDcQaPapW0qiOACxg=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/e5LfhPK3dX3G0A64dS8UCCKJyNEnrt5egaCDKEIXlgtTTz8OXAkX7Is9zsrgXNpvrSrVc3yybXkVFVYeaU3LlKIHDjKrDhX1ObvTeDgxUisT9OWrj0CLjl0did4O4mR7-aG70Bx0clfsP7_KE2umqn8iCTljQqBfXYUPE9nH3S7K7aGR5n16GeIXyOTJIgYoKbRlFG0tA0nFCwTYlKJkEx3u3ovCo2chWbsRRrpj122zP7nD1gS0Y-dcALJBVhEZIexbOGBkP0G6FoNzczbUwaAg39nCA5Hp_VowAuQNFS_2pdoWUAkVd2EBC7UefmfrxZFngVPv5X8d-9N-bWpS1T6s2nS4KRoyVLMoNQ1i8it4cIkeb72DxCV-NboSvav9BAHVr0uSrMuz_krFzeVSH5FbLehyKsSJuCVsNOWkMcTgWHFVxLj9HC6iT2iA62y1ujvB_SDD8tr-hNLk2gdjIpCWvQYvcF7bSGpwJlT_yTqItjtrefeybeypa-Z_fvLgxdLXBpVFkA1gG_lcAV2tJ9fh-oCHYllH3gu_O4qXcMPtSrJ-BnGLnauNgNtU-85xoEFT4pkmBvYB6hhJbZ6o7QKlGZHvbMkPeu8yRO6iA0BQKLrERBfftYDw1gnGcrI4JOHCwu-n-0RAXgSRaxvo-JC3-wmOcwhvA-pTitv3DYIGL4bIRccCQpCrKOjzCg=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/XtJvfCU10XCHprNUOAKaj_qO1pgLXB5vRC98qnyKxK9xu3dIwL1c8np9uzA9FXAy_-ZagoZ4NhrSkalYzhBtf4kbnD6POT_dz9YvSqJmum7O2v3iuJSVF4WUBeRtpoW09P6IrF1gs7HKAQuQ0iNsuoKEZmDlgGzjrhi1YKrSWpEZj8D0q6v1Evkfx-7CX7kzuDCxETjmgjHwy430HNdRzmkDgJu9cQiE6zhzLeoTE7QWm0W6t9gdSB3eijfaXuUJKnkoppr2LG_zZYyRDDJA_GIlfADcWAS7alUPbxWqXeYP2Kr-X8sxGCqpyNxvvgEhfchAECyVoT3a81iXGf5yuha05VxdA89A6wmxZN4fNO4N1nUVtHUElbj5c_-6ahOhfwZDNDyoSs4uDrIEsDnGS-x1RNgE-oAjIhbDNXdImQJXnZ217cXlwSIgYjO1ajpZjooR_CLmdAqWSKALVsrGUz81ni0QDwgYuMTvwP9dOBoGbm4gJdwyR_PYOxAWAo8f2znDzAx9tjw_TxUCL_iQTPVLVhLSsmtnOQWTsUYiILIkQAjHRSRVGQTX-Ttpk-o9A_Agz5l0CPG_vdrk2Q7vgYmIn9EAENII15WLUGYyTyhvCog_P8aPL0ewAxPbZTd6L6TPzL9pVQ-ldEdBc1j12Gk6wJLLJgZvduT3ZS5zTVDyFpV9dCT89ZLJghbROw=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
     <t>Our old friend Jason Pham comes down to visit us in Blacksburg and hike at Cascade Falls!</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/_kHh7qGlYsz-hxYnmoIh_yR-ggt0uWX5s4u_JcFTqFux1DzYnBTvsU5Qyw11MvbxudeeBGYOwfATrawOtVeQ-hphhDYu92JWIOjmbs63AbUTRRs3sfeGqkNQ5Df2FCAmeQWujagmQpf4Y5c2gAxU_b0w2ocWxvY82dNL2AJ-r0p6KJmkTFTnICy2s5rLIckHV4qRBvwqXrEYp9V-PjymKxFj9hTM-ruVE_-WnX_eCkMgj2sXfHy3kvrwyOvOXnsz8gy0SW6xwK6TpFVAZbgxYaxAvpq2gpAb0CAw9_t9Ve-vAZKaO2_I95b1FpvfctgX1NVCcLnPyltz8rdWPN48F03xFV4YvOMIeenZPUuemzHAcDi4UsfViBmBQMzuwVVQx7Q1pmSDfCyNlBtn4SDQQLVDlP9Rvv2qisQ3A-g8OSEO8qObaf-Zzg_dFzFWaBAj7Xy6fDGpcRWNpSYcVcIZwBw6iuEnlSaP1k0OpimUDzZiZ4RNDJwwlj1kRIYgXXXZZIctXctVQ_NX-TpRoByjGXeiiC8TuzQ4crijnJVV5Js2YDba2gU-HwaVn9tWXO19sQKB6SdFTiX-Jl3a3j38cYon_49OgBbOOdIWFKdfG9dnKyZHbjxt7SuHcagCOHs6X19U6ReNk7f-nbmJx7eZ6i5XtgLo4Q-TOa_f7RkHaU7aDqEQ7XI-8o61ZvqMTA=w1048-h1396-no?authuser=0</t>
-  </si>
-  <si>
     <t>Our first time kayaking on the New River!</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/eFHQtqqkke4lyV_ftYOz4QQKETn9qwHXnMEOoKRE4OAUoj7tjZEgGpvMvzcGtYEnvxoX5S95R3cdksqi8RF_wO3msUkcRueOBAUr2U6ZYDzzOnEGanc-OLCeWtu5JuA5bXip6KW9T4XD0XjFhO_uBcUBnY7P2UQMYjDbSLfJ5m36fuSGCxKwfRISEE27j8EvA9VWAU39Nx1nXl4jc-cAdVKDwU4okBX9xp91N9NTNmCbucbYnyLNK5NoWfqo5ShsgmqsHSykMD6LcP7McRlm35kdgHRkYlUx9dqopoLYCVMiJ3rlXzY73eARFHUQ4I88fWNRmbgMyX-sXzuIRzDBqrKu7O08uhIZR5kHc5qKOYZJASpNNn1NgwEAEEKQycTUaoSJ4gAtNPzZiGEims09-ENT40-oWr9UPMEaek34BPlaEzmKplxZuFlfFVessyE-oBehaGCDR7LTqQgVYgDwvJ-Of8QuwShPlOkXMcrXdZjZNLdaXwjavS9NsiFmXxbNDDKK68SOW9qTSLLG8YTBSjkW3_TmwvQZ44ITnONLNOoVNtP-2wZQYv-Hw8vSPLFo3E7rIydRx1BKXywyDy0bxHV47v9mNzEBy9ibY73cAifb_Piy5gS0kB6zWtf9P9y4u6Bbg1gBEfn9ozEkUcSytBeMK4y_k8lZBnA2QTebpf4aJW_WwxSAbxKSpoCWyw=w1048-h1396-no?authuser=0</t>
-  </si>
-  <si>
     <t>Matcha looks just as happy as I was.</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/7DdwlbCpy6AMnGUH9KYH-IX5ifrNT9q_yOlqFc1hj4ti4CrxB3OQ91xzsL8aOi-FU6VG8FvqFNPgbI3wTq96mXC1rEMtCAheTcNQ3ofcs2Jo3PdypufUhcLpcnWH_sY5g7avqZylRYcuQBjSuUI_-BeHe1r3fZdFBDQXlr7y45rWGn52RDqKmQR6Cj-ZkHWTHRPjtHSolmsCT_zEnjBEnvpWTzJM_UjczC5uHQZwy1u9M64xHrgc67kdOfgKgy4IjFoNNyh1iI4KVaSqfa-WXRnMzeBBXxzU60U2MMnb3ryOvsHb50y1VGAbokH7y7fwuJPjnncW7iPT8HBVX59j1LsvsRQY-QbjLLF4THORp71hVJnMEi9u2irAbNbLHQ-yYnmDr4WraL_nWOuXT42BLCyTkrcfzOUCXaxQgS7sTk8bxA-HzQVo3xmFMFo4eSpRDjJhRS4JeylcRkK84_r4Cd3tLfay0v6OSp4hQGVxc02an234ghaY7hn0XR0Hhx0zcUzor9rrXH3ZJSQ7dpMkXNF8YiEk_ftYfVz9UMntUjk0ewkxgCHatzKwZNXzt0HbHstN4Jpy20MIE29avVbj68ET5OZLpmvokEgM2QTdPBQyKJAVu3_KGZjbQn4-M5hHxxrxkcVuJQSDwcTgx9VcEsNiNTQEJqp2f_Hs0duhisKVJBZs8w15DRSROf7wtA=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
     <t>Our apartment complex hosted a Yappy Hour!</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/yFm9h1jOzp7kctZ9Ev0lx50b0RNWRBmVSMrLZ4XGcZ4akMHyEDjfjGVvYYgydMcdFH-UMgJMfTrLzO-yGQUFAJ9l-68QlqAlwl2QVwxP-odQQjJcOU62xTekgLt27KLD9apXCTBUa6bvD8lzmgaqcGmc_FIJc2Lg5kAVIo7OlsYCFxxGy5SSub2QKhiJ6hfKhgojPOjCeDQ38glfVmdnAr-Lg0FZVRWan-YtMWMD_fwuGBAAhZsWtpT5qUKrXHnWqNcDoSw07IzLuyA3LIOYyp8vbdqNHxD2dI0XQ_y3EGTxbvYqjU2O_vr5uDXaWb8VaPDeRRa8fiUJbVaa0tHSMzvbuyDnZ_CcH0543tiMtKXanr95n7DZRKo46Zwn3x15BKUH00CtxcsOpa5kumbVlqUA6wRSDn6cooivIojBrROWJtirWXBaSPdqXgSvs_qnftnnjT3da-rDf9KFPKalprdAmDYeROaOvFvMz7fLqA-XIDlg5m0eIMGwW_5cA1cXzYhF6xLH9pFl-LzM52rb3c9Pgsra9j0efFa5ikenzg6iRVjFCZH4Y3_CdOj6O2j7NvBZD8GMGlpr7L8Ry06bVMwpa4ur4gSYAcxrfpLcQpUOb3geAz2c2Yz7mB8VQEjd2GtTBCLa5JlV5wByFyQoefJi-6G2z-s1ctGZSV1O-5JQ7JokjoPYvufifk5IuQ=w1274-h588-no?authuser=0</t>
-  </si>
-  <si>
     <t>He's a very proud father</t>
   </si>
   <si>
@@ -199,24 +146,12 @@
     <t>She swallowed a sewing needle, but came out of surgery ok!</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/0a6GkgdUgbDItBTH4LOzqpScoeBG6QRC767x9oo7r-JA-UxOFiMVId7eAZScnqL0yQ3KXnG_Ct29pc_imog92kaO1yrBHh1k5_XANU76GxQis6ng7UEtFopT0WIeTRmybJn7yTgpyV65m9-f8W6jf8uxZtHi4-4EyYbW2xpazdhjR0xjFKLT-y9smaIhMrqmY0fSdSE8J_537GyC0rMbqJvEfGpx0oVwyu-5YXpSNgKxJa8QYYI1lLizROzUubpG-Y_qyJcoAzJQwYkZ46T-cpZ68hOYBB_PDIlAMunFi5ekC2xIEkjJz00HuLd-2RlI-mtWZ9oJzLt66yJ4kcuh1kqM0uPPVXcSPohwntFwxBGtPJl1LD2L9cJveBQUh74-AaVMUSTHgpkt-XRkhD5iXTayz49qXQnIC9RlvTlr-WclffMrC3i5gf-OoQKt628bdjha-h99DfPQEN1JWMNUpEivNCk-gLOSTB8XZDhFPFmXqb74FJqj0kF9yF7PKv4PyL-g56e5UXQC3NQFkf2gYHAbjPLdtDdDYSpiM7Nr8YZXYDCIJnRmLhYpUUgG_5XHxTVSHhwQ0nQWcaAZiHUxvwe3T1gUyhRoj4CJAX-XMglpGtOlH_vwbJutRVyQFSEHv5b1T50w2z1dqQ32Kmc2etwc0xMzT1v6omi2_9ca_1Qc5YlYJIX7A1ybqiKEvg=w1048-h1396-no?authuser=0</t>
-  </si>
-  <si>
     <t>She came out of her spay procedure ok!</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/QsWCMC9C_fQrV3iQX_A0hAsHb13ox1-Xn5MjWvxPZTzqkVFuQbDRRRE2jXy2yEGJ_QrL8Z-A-oMP8qNX5A_sNtXLPGN_OD4zccgEj0QqSqruOUKgDXrUs7F33G9KzM2AFxR2zCV-Y6GuqBEN48XJ5ImeH8y90VqrONh6BP55-rY0CsLAOrq_-zk8McWIDtuS9FfYda-vxs2Hm-zCvalAqr4kp__fIhmgC06ytXJxPI0nJCkBypE9u0YwVEQ3CWtT26XZkHObqX-GHnuW9e4OpR9_yWH7xuxEevGpF2U5NtnqX8d5LQ_Ue7MAmxMw9QN4nEJ1yq3dFHNm1ddyQ-I71pHFU_Hs4WOyPUqjkHUTYQuW_a2CSM9z5bUut1ItxP08AxUsjpTlR5XI4qCSwAyanoksc33aoSW1aTT2YURvgDu2w5DFtZeJjW3Ph4vjdbu37aTIROq6ImnN7gW-nneD53LvPfFvl1ewz1kndxL2Re1qyFs69yZl9yn84AgDFDQW7ZQilL7k4_j0YH-3WqPm2rKgfLKJYVQLp4TcecSgSisSGiT3ALKDdJ0JfK6ozinOzMaITT6FEQhRpkNcuZOZBFocWa7YVlJskOdCB4lF-EqyhLx1tWtgR6jbv3Ti8StODiOkYX9BOdYdOuW6uFh63r8Lum1dj-va0l6oj82_SWhmu7yiAuYmhbYZvZRTKA=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
     <t>Matcha enjoyed hiking halfway up Seneca Rocks</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/Too6SbI2tVRrZh7uJHzPTYNGbaWJQ1ucD-4rBrGwZVfazgvqSKQDK7Jw_aSCngk4wzWL02UQlPbYSLbpXL4t5rNqraRU9_oMi-lEu6l5Vxche8yKYL0lwDNRleISboIAI8Rr99H_EtUi5NzBW8fGcWn2JC950C6grcjH3_N7DF9oVWePZ3ZQgkI0IwK06nalestFbceDOC0uaTxwZjPmmBaWcb9XLd3mX94oEbPVxaE-mGf493Ez9Fs7yb-5crLd06MzZQjqTpITJi2-IY_73dzRkm2X8n3INbH1BvNrQg9-ExFcXYuzPh6VjGRSnuePFkEM8OEYfrAbOCV3K0wKbnKWr3QAbcIjBKW4VlPoclo_W9nYRAaRAc8nt4Wfl9Rics_MmpuG77NmTTYcS6CnD-v1UL_4EG0qJZgv0gA-HMbR1Lq0fGQKfYkrU3S3S0p09-7hoPZOXLo4pWdzkeHr7a5OijdB34NVGuEnaHaPX1nDKERQvffsl0uHkly9PSiTSTiX8b2_pbnQzuy6BO9fXBM5wNe_7feFd3R-XqxHdCoVHsMeQIA1NYWTQPZWuz56mWdXsdIpquLWhh3IM9JLZ8NjtoTgW4kHox9WvR7UVbbIsx5nqm1GtNV1HhXf14YsEetluUmo3RK5WDvmvRcpJCHV3HJgqTVX1H4g68twk3eZuqVLMTyKEP08a2-NHQ=w1274-h718-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/HTBpijAIiDbJ0Kg2ps6MCInpbDhQTPCq7adLmLILE7LSyql-BcusgNa0ZD_k-TEuS9Gz9vWrGLgz99J09OMZWwj8WL-KOxdEJ855cHZwiM6f8Z85A4VBxI2kR7S4uMncC94myUa1R0JwVt7a3HXMjAOTk4aCz-1DAOFQ16WUn6yFxHUq87dTJRwRvVlcKrbrIxQvKHIpg6nYAPUMDbJNedq7JeL3HrfZvCvmfchWhfO5tnMCew8pvMDWMKSZ9Vl89a7GU0K2gZUqZMaHgdj02t1FQllZmFXmJ6D56KeYaLlAVTaInNZ9nhpM1ae7nTlioBo2weNOvKQto3xD8v_MX1xL0WFV6LzdaKAbKo9pA8H3Ws-7MWFMhcYJ3FIorSBsKr9j4s9p8N471PPzl6GC3SfbT3kKoAsH3Vdg_d4UxEbufmVrh1_FNGaghOeX6uJiEXv6osrFUhgFAHXXJc4IkQNnz1olVTivzm1anCGLqfR3QLicy-0p5BfzCsikrGMbySbrQwYrZWWWGa8FQ3lAAVJLejhVmDOJaYvQg7zqLLEOmAQjcQQ1sj9GTDO38CG2gYUt6qJpR86EQbt0G_WeD_KbGtg1o7bP0s3k987lpRKR2hRUgDImv9D_o9De4AV1cq9pIAdtacY--T7L_JpSxE45P__zyndsUIgd2HaWZLMu6Yj_X40-thP2H2hiAg=w336-h252-no?authuser=0</t>
-  </si>
-  <si>
     <t>Little Devil Stairs</t>
   </si>
   <si>
@@ -241,13 +176,85 @@
     <t>We visited the highest point in West Virginia! Afterwards we camped near Seneca Rocks. The trip ended with a visit to Luray Caverns.</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/ICR-H3rjrXPJMUMRdoyeRxYwUmc-PE3Hg91KgPdqiDK5x3Hy-tz5IV7YhZo0Y7ygcADLr3mYDjCFRUFmlQqFDCA35KdXMm9c8oFMfeN4-4IdyRdlloXD83B4OtuJ5ua_OuZDFVeG289Y3u0LkK3f_eWntskeRrRVXLAxlCPhJbIBUoCaL7MSBs8TvigBshR8YeKoGnFdsARP495EboFfXjg9-ywqcq8LgXoaM6fdXOyAU0p3xGBEb9jLo99rOYrfYg0z_B--8M5B6_o-rHuOClZPVb0IhO5CK_1IGRlKDxx7lGMQqqkmRWcVPhlELXpSHf5dWs8BLmOAqqBVHqNzPXJtSKh_RCqy5-zxnl9rhwH-nYxnq5tazRKRm0vzAS3iOOvfDfgc6wkapYWgyOzMRjoKsyMGRKO_diDGpo043IyxJRoqdgDqklSXrxP1dmMXEKsYYfSOxZlPN3JRsjI_LrMMOdP4TukmR9hTZ31I3CMXM9Pg-nXMYP4D0bHWeyadl2zEZ34e7ru-1fYN9OFQ4uAWi8drZkGs28cNtBsDKMBY0BzfXFuzpTUdm_20Bx7xIY4PdovjDeOCPMykZ4ZPHao8ZDLmMQegmU8F-uCi-Mm_HKDk9Vq_fveHXzBrcHMDwh5SemYM6RdAKXjrN4bgZ3qnw9hQoFq2CT4aCm29o5F2xEuAnVs2zSKoGAz8Ow=w312-h234-no?authuser=0</t>
-  </si>
-  <si>
-    <t>https://lh3.googleusercontent.com/PWeCFi4Ji8HJisVP0udLQLho2xy9GHDOY0wkLzb87f3GyWUsAwpEjdX5Woi6qihfPaOAfhragg0Tx2n10-nvpfIcE_iP3u-f05IxAwenUeopYK63pnWSGzv84TqkDAIPSR1Pag_v_ODcU4L4F-cMgDUuWMn8g4iUjwoUBqxWC3Db5Um9sU7u7x-_fUf31RX1NPXaEaCSL9ocl_P0g-QNM5D8fswCaLrTGws1z_okflMrfaFpWSn3y15oOdXXiJ9hvLwyI9VHtYxwly-Ti5B7kOVBW-lWnYcKnnnUiSn6D7PT6wXUtLwXxvwH3UPlPRLy4rqfUicHt6zz3mGhPwWVE-Yi1ojT0qqvnDC2REwoLhMKvl8Xw9bE3S_5n2I_la4HrS659K2ttiMB9HVn7kDH84tl3rqf3KwOxSgrpn5JhiS7hbew_BaEBVjyhGE2xQfpI8_emr3FLwlAwLQ7Fawn2K9FXn3VhwiJDjskOpBx6tHW5ZANzeynS5DKSjz7EBNhi_-4OwFXndgt14au2IvoBn6lZFnXoM-fbkVGpW4b_bLXLzOErr1brnfkO7ZPwVwci6y3kavFp1psqEtiGOt0nbvJgK9-yXTuQ8fLm1XSAHtjFltJPkiQR07aNeuzK-bG3NuGJCiYrD-lSTc1DSMOaV7Z2X7ujlRZ8RtHnsVafBEwq-FbymccEpuNZTYdPg=w1274-h956-no?authuser=0</t>
-  </si>
-  <si>
     <t>We only made it halfway :)</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIrvxvrjPvm7eoDKso80lf_W3LAX3cdFtdhjribuAioj3Hcll81NhFSA5G0V5cEf0abcNEE4z-CuICxVlQCUm8PZ0dyDTebfrMYKvrZI1hLH9w9cBdv5qfVz6jpSXxPB2DyGgLQIOcJ8PDVes0jV6tFgUNRq1HF7Z7aOg1dXmERIlgLtgfxES5pNCHGN9A1EAs7Otq9lu7XiMRcgS0BH1xpZGi9AnteE5RqSseGUTX6gMG2XYOHx0Gx9C1im-2kxrF9XchKCMwt6cvdriSgP18HC9ECqVZpZY4owEywwb09swOD_DprjDxJtQDn458Gj3zw5K0jwIA3aQBO8CMIbXL1dRdKtDhNrFwyH4ujnQzcoLzghasH-F3yxwgqECHdK2ARLF-cFvKVsNnGd_dKAssOFJkbdoiDJwBBKdFE1aW3-FQb5XWmNgmsMGF0b-4OtW0t7mkBSOff0JjX4318z3_PH7UU_T3SjFy309KZMtJTLapS4qy5M-5w0yElZG6h6O6ziBuw-YNE5lXOCf52ZeIu5U_SdJS-EzfwU9gEMckLT6FOxNr3g477HCAs3eJNazFW14FxJuFP6lrLYr1S_kB7h8IxEUyLlqrZjtD6vVWe7wA6nwyW6AEOPF1At7f6oWLjGWzBPGPK0qqhZ6cY8yysOpORQWRYrXzYAiUzmOqToymdB4kXWFWz3_PsnXzNrnqWdjZvSayw4NpkIBQa6mnGx4W14_8UURUc_mA=s1274-w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqzkZAzlPy6P3clhKUFVw-h6zSEYc6MJQ4WiWijH8sCzOk2JjRzrpbpmXkCj7Vi1_4dXtBCWcZMHgBdJ7r4K72YNUWUxC9p79V8I1pR5E78_n7OJSKQ_l3xu9EZzpgFv7tbt9hgxZz9CvJ6q4J4yoRXkBf_LY78GrOrXTRnprgxEmfi0GypLIfFqOj7Ys3PzsvcQ6ka3hl3mRHF6RHb6cWYUxlquz6xO-Hk45emW4aDafWKpXx-nG8_P_-HwcmueZejg8TvY5jZgSrVJOHXTJvIATnfNy8N-ZdrxmLN3yzwfBaJ8FsnTsvIsSMHiFJyeYfnPtOIZ7EiApxPeIfYG-DvtI6tezQQ-RuHkH-xTRehCywDdnN_0ugKITYvuBt9Y8ZUnW8I5-YauKz_w4myGR_ovDJ3STmBuhng0_p7ERVFducfpCOgQVPEHFptmC2UC5T7JafiVymDZRtgrXZtuNdhx6y2AFvqM_T8FG1kEdnqnoRojLtdocEiYwJ2Pz-TDBnAeA-lv-WkGIlENcA8FSo7TNj5TUsUjoMJrZRwhqnwKYJRlWDoFZApO6k2UCNxGSuLkhKxYAW4uKA2I3EPxtj0lVqx7-t09fptE_DW1IjphoS22rtjUbOcriuaAWEneLYpmiRD1cyzT6N4mu4vWS0oBNA1jh_tr3khGVRmefEWsHET26kFoK4D72t4i1Nfs9F_5jIjaEEJPPOrbtAdkXXRYf9uxtKMdbYqFA=s1274-w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIpC11vp-VIRFhpIyGp99K8VJnXh7d5cw4xhcfo87gRX6cvjRnOODCAgHyFtU2EYmbVrVqELS7KDD_qtDhIiVObPzkcdxvTYMfX3S2GpRuOjvk-xHEdnfd7qwA9nG1tPsqx3FGLkm7f8uVFpNKprCGXkD89iud15gYftcrNRoEhHNs5gV0WZ7yRbEMVX02lNFdzW9FI7R0hojP292QV3hjIjmE4aUOOVZtjWbH3qtpRsVl_l85iK1CyI0ey10KbBxPmqn8Cv908vz5oEUZ1BEgseSAq1p7mZBnJIjBmqwWAuX344iNv-gr_DrHb5EKDcHhUwGEKk10jRFYvf64ZwNhaguljp9I0DNsZfD9XaKWlBmdLz_QbU3R_2Qe8urTED7FU7UeEh4pSHNRTMS6O1B4pTzbEk0dq8PGASyQ_dgwALFRR_GMQ4NhXqxBYZ_CURSmyddyf9SAiebpwM49JzYcYDfVLRdjPcLKd4zgCq9TQgz75uB_VKiRiuKIkOc_9hoVgpMkWweA5YXeeE9ZSTaPn5Fw0q2fzoBgNcCCvTkFI-YAmoHF_Yq3nnxRlzKXeLKmlzmjZ1LPCO-AIJxy25ZWDGLWIJUjubm9gUUSaEtCAgvHIzrzL-yPIQI7ShJkAmB2AeeAWZ3lmPnqCkHb_DgsibyKHDuQrOjbLpBX1tzGLflgTn7QgVXJdhLtz4wFjoyeqIr3__erycMobDoooSlTSnFBEytIa3xEGWvA=s1396-w786-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIroEyiR-clcUqiGcnMo8dYWiq7qA2ld8pVpBCkhj8zxbXdENxvTAu7IIZI5Wx2I4K9NwTdCe6WwOLdJq9uSOPIhcIkFZPH_EN9yhTZJnexlnBu7Fgi2oweRJSFPJPutSB4_K5grRTia8KxIc4crvw3ll0MHtp_Uu0XmhhS8URXXKoYs58zLuOUpmwGV_v2MPUbG-ZGorIg614wGRd49oKBIQgt3qrUwLsiCbciyhfZY8GslGr1D9usRsavVw051b6enDh_pUL0yktQ-0i9t7vui4sVL8VEz0EmSvdvWWCqbP8EPxG9oeKr9ElwSxyBIoTwtLC5iSi55l6uOb7x3olU-KnZtJghl19zU_OXCXv34E-S1xudVcQaD9MYCstKULx2x-SHuI2bL1oo8tojn-z_8Irugg_ZHmgww_UIHS9PcVAdTUqv4vISeXX0PYPWSlxm0ppZ_IaV9nv6zS_bgYLk9y3E9I5ZgpuaxKUvJVtpPX6G-JD1ruCYnKiIvW_ReSSnYu-23IF35qk8hv-iJmUK3WwfvxpcD0it-HuWYhjZWzlWcyFztFk--KZnh0_6TktsYCvad0OXlVYG7XMbR1pqP-Mp_VfJc-olhqpe-1ManglKASXaxai7fhklFQKOw2GG50_hrAnPNUd2XnTAOfAXyLvi3BCEYKVZOfqlZS2Yef2Gnu93_60I1OEJ_vKCwobb2aNn7k5fcxuoz5dM4IV9skxIth9Q6ChOp2g=s1274-w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIryTdBIJkr_jx-9fZBofGIMfWZu3kbWk6FWUsnFuLQCC_l2gqXqYIjiwnQluNr-QyO7qSLqs1YXMoHVr3KxEjYgR3fCJWfkw0J-qZPOKzpDGy_TjxNdpBemWedKZu71SbOLNNFXmuZjEidJZUDUUb8i1xbAj5TTPSTEMjQGgWCbAyhZgBLZSbwePcExT0LK8-8cOhaFiCkU39tc0ER-A6LRJUnFGc-hK0CZNMf_yGd9ZXK12HSpQUpp3MbBHpjRdfd1gF4oqTIVK7FXw4W1lLAqy1vO-HoXIGcb9wmEjsMwotaqTCVTwtCQb7eiIsgPh-kd5lrrOdIXMr3wYnyACbXRZ2tvYgDg2pP1yLYGscMyR2ADqb0n9vYjHlllGl7Pv0St9hCutG3csizkSSU_nEHAZbYCP12O_HIWcaOxOjlgUk1-dkiKd7TxTfcqZDnHuselETVl4Ngwp4M0aQi9Arsdqeih0zr3SbRRNZZ9ynm-ggtzPJoFp5WjYGBqvqOtV0Bnq6a7MXEGfDhBjz3VUD1C7YR2-98hivswILlAxMgG3FN2YRygsw_tP46i8Xf1jvtyR_2yo2K5IV88D5U3a-QOrs2FprEu-419tvvsUrGeWIcTQ4iqWkEKhIepNdxINs8od0oszq21OhVHwIgHavKBGNE7hRxqL4HgdqwRf-QWNwX6PGrA0L11j6F3y8Fjxmg3hu8rTU7EGBaiJADvzAawQfH9PbvkH6Jcjw=s1274-w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIrixYSdGwGVJF50fCto7QesbYqOhpgxX5fhBd5d1eRElipM0B4987Y5dtkRrpci5bcffBIjsbpv0ptlciuaNlcOvIsD2XlkDIo2I80aLPKrkCS8KqqoAiBS1O_l5kBKmywY72MrUfmOTxmV2x2EG4mVJKMlR9Y5JmsuccVJbPle9PO08be6Y-NWJx7bhsh_7GgTvkpL23lm6nDtwQsGAwUxPHiiBQ0b67Umxh7M8xZO5mApnuHDJUXzww5hjjiJr5wX-lmQSQ_MypYH3wy2zRxoOiMNcdSYPzgHmaZWFl61qLCP69Q7e_VdUYGnJD5tmPE0-SmyxQ05Y32zcJR76DvaMmf4glsBX5nE7-9Bb0RCtjiKNC7Q9MfXnXn5JVwmhVaxz0KC4P07AoQcsOTTrPZlq0TWCYrsWCNgkOgeoprTKkealciajHNrwXT_TX4mrpxYRP8SoXl--6nFMXbJre7LlfEbw8NoViUpwgbwMAypdHVXNddHKSHLoHK4HyeZ6sxEDVuyBxtjPHX_qmGaWbXBLLJoKcgibjvmSanhVDugpgtMh5tad5kj5H1DuL0cadlqPGHoz-cNM4-8LdLrBEsuUhy0IlckBFipsFTCUijuZg12JekD6T0_A5F7AHVlN6l1ulyW_06E9eDirHKl08GOyfxqO0yYQwb54NfGNxgxZTzzzIO3mZ3vl4gbede97_EHVPNvNHITXjcVn0HmpYPgmFKQXlkq38H7kQ=s1274-w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIortV4aRQLoJS4rCbcPwbfRpa45TbbDLIlOp-IJglwpjXmPLAloc58b51mcEOWSlgiBdOkD0AkKL7c7wKCIfMb8y9l-xqx-g_eRDU4sFRbzdV9LZM8coJMiVrV7h9YGNjwf6IHNBbA3f9nVIEEqVVUPZbtrLYuUDv7C72GfydvDwAVTzZIorD0DIA_KIhA6PH-pJ7CQUYOcQdEiInnkixVJlmG9ZQovmNmwzNu3CxZkzXgqo6OqDm3ZR3-9O_ugJnX9eLTV2pmAPQP5D5sKxeOFsB_eHOLdvqs3O2Ikluhp4nom5NARc_QG_YSX7HkygmmJVypoB9_VfW3dBeL8_Wce9DLJRIb-C-RtxpWSjcLbKco1xCjIZn8gZcmzpSWo7U0uCqPwD3vFRWcMCnXlzD-3tT86E58siXDJt3AP6hAHj5BITNVOEgw9bFMn6ms2bn6anVec7dIXcAdrM-n94VwTfz3xV3TMRu31TbhhtfFsH9C_fGQj6tIHSodGA7Dvx9P2pG8mYLaPFWlvNmluTj0UKg9qGaXi0d15mhOUMs93ss4Y3cTfT2NjPwjIPq_giu26_YVJPZtnManO1Ho3znmqfLAMs5FEAkT7CzcBtrW8038tNxzWJ4qE4pYlgmjVis0hwtdDB0oxytdEgIZ_Dx2qK3ikjX8ZYv92D5PoyuR8oMK2_S9mBzHB7A4hwhi04HlpslKyCYR31fTv0qTMKJlZR7I51ri3TgJEBQ=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqYhj5opn8kIGRCP4DX7lZ8o5OSHFh30GJBck37U5OFSwUdjV9vv0MiKKHky8RNQup-mYpfvyV7fc2w4RtpilS4rfoeV_oh-NmZh47epyJk6MBFwpzsVBzSkCDV-j09PX3v6TciU-S4Ne1TxZfGxvxZqq7k0jKI7JM9-JoecgyEhR7GMyzelv8sNfin94601MjtjCa4fE3dLt39gJkp5ESKeMykKa3TpvOFmB5s7_ns5x4XiAmfm3w_NAQjTuNk7F4zfbjTmWhIA9A1cuEGO2kdS1_H4zR94xPHTv48RteRkNQPPsHENB_pwMll12AHtqJIa8rkT9RlZ7_KggItsrar7HBZV1-MrV9DcSRS1pl_vroiKGGRzsOsP83la4VTgBHBsb8AIiNbto7viQOP_e6ayw7uZDLsX27r5tgM3sXLGv9dhIOzUlkqMN6Jr0EctuO8qErAotSJU0K3pM3i9oAKtKmcAFvZY_kWjmQ_CcQOAUw9MViTCm6lRO_qtGI3LfvX6VRhA5dGj3Yu8ZVuQdIR4TNHFHldxdGPd74oeXQI_f49YNKcrhfID9aZcq4xhv5UoaKfVNLzADLcGd2HwFXmHntNWj5AYU1Oi2-1OtimWjYBSwTv1txq7JmRXmbtBAqfeML6a65zDqMz-In-0pKHKX_PygTa_QoDMxWt5vX63LMPFCyCGhkfjca41MqjuiNqRKZ4rDJ4oFN-Gb1SZVaW98lxPd5SNp3h5w=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIr7Fy-oy9JZGmZQbJqCYMcO01SXDbBmEdXxDvpPnqmC_VEYTy_ME9yZgJWS1STbJQ47za30QxnD8AGyC8KzYxXKMu_0SQiXaPXoiNO8awU4OMBT-owWQMGFsCtuU5jBc_Fz98NLTp7XVxGVgakCKR3qi6xhqkx5CbE92Mr04DyNdsLbHCN25i0DkEY8-ll9n1SUnxIcqr9KOmokP0-RBseuYefOmseykEfACIC9kuBFGKqaWp5znM2xMmMFBFxpZlZcTIZbmv8MV_i1HmU4eO2rz4ppMNNBXJ_NBXgiidU2D4hlNyvTMBW1cbhtJ5fCVOQTJQ9hNd24DodYQjjmr93lCcu2f4hoNwz0cpuDgNeEn-IzRJNq_ESo2nh3TXaruITtfnk3iHebrREvPKN66UX0vF7x1xUyOqM4Gol08EMgcwQx9jouYmwf8aT-Qvkhbi8Gi3aWNpxXrBVqI2iBJkl48Zgiw4-xjbA7nYMCje0AKLThzYrg65Plt2qhPkhaB4jncx9HAB2rQt9Pj4-YWYydX7bPt1sBJx6X5JSKO_GhkNU_6Fs1P1hyjE6hAE_qy39P2A0BboDxXKI6FhgeWXH13vc7bQJf_347wjldqFbX4JmOt2Den67EANA6rCYgMVN0Yjxj2ucVf-LgaypJ2raCUAtOHIbReXoW3BrT9ZWSvHSjROJtHLvBOY-fLF8sTdpWspn0fhnv7FwuaLyd467bKcaBRTWJycbe4g=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqRgKybPYKW-TiV8mTpzEK2MCqHLfUKhEYHF4C8nRPTui4YpGqGYiSK9B-f08Tp81gSZH7RgYrVu4h5HNqlqzXk75-7iRt9jOlwVvpH_3ATL8p0CsMV499Ho8KjqZaw6Jc-76GOgU0MqIXnTpZJU9XKhPlzr2v25L8FkKlP4TOdTRoDTl-UcomdJ6mftGiFNXvW0yV2m0n_TsuUgDnT09LbRBDXubLQl7_4y7DO8JdebjgeRhcqDHu4iibrGhGczdr66aUGq3GcMn1P_jnwRw4CbEtzRs_XT-e0_DDKgVF6wRfqDtxj4CUu6nLnbRWZBlfz51VzDK3PD8l9YTX4p5ritObXNeVrFcclZ30pPb_ZSpGwKe7_6Pi1JgEq1bKdv9FJsy1HVkKL1i1Z2MMBGio5IrLTWZyMXDzc3eNMlPI0CjM42ofLpUQnOHD4ea4MBhLbnLt-PzQ8I8AUIQKgxAzsfkf9m96MDQ-ToRvFMHGq8_cRdcXAMCE5hL4SfWExYGc_tDTpg89sLCmOLbkdr-FcbZQnRZk_SiScBhaqL76XkOauPPYWUFO-ZwbaLYHoiq-HgOm3bPjZMgYxZx-KdH18VGgQ5grBXFeMCI27nPZIiljhu-7kujYSqURGUIGCc9xRrkov0HC0GV7K0Kebq9Nn1KQSHlkEfq92sxED2hlyHYKbA-X01e8JXfe4GZLPlrVWPK8T7IQBvYJDPX_0hCNBc1au6ed3-c21rg=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqekLsDJkxvNt_90n88jhxnn4m1Vt1kQuu3L4KjCpQVGtGOaGJFatuWrz-DVjrKlebDGRvfr3V8z6VotMz3Z1U4LkB9lMEz6OkbeQJFX8CRFOp_cQjsltU_a3juraZVI_3h5c6u7k4-xP5bHmvuofWhvSbGFPWUayvyvPV3iueB6WMzdSFyrUDpTKawygvQdgBBDVdRxAwpnANc_J6lTyWboxa13emEt-XT-riujmGqU8rYlDf0GnMu91JhoD5b4hV95YiYOXpkqkdQPXP8uRdmqdpRUQ0EAEAS6o-sGbz0zU6RVtstSpZlY8lscopkZcR3hCQeu0sAUL86vP3HmOsrLYC-R1CPtiuqbN_2hUKtx2QDMjn9-rSKh-UN2zeyAUMLPdfUYxm2h1Zn1rciknRaRxJ_Vuxm7caUVa7qWSIC9wld_ltAyovhj3kLOfP_cCcW-Uh__X3q03k67bjRbOz7otYSb6aGPVM8NR3w5CtBTr-8tfTet9XBK17avOzish0O0I_-ywPCJ1ES6gZKwgPzbLy6nhGR5mUA6Fj4De_OFuHpgPT0nMimB_BomQNkUyzH-SBCA5veBn4h6M4e2B7T6T3YYQJP9ntSM7ko05JHHmpWau_nDMsYj_QH3bs6hRsiP2NmX0ZxfHJuQtVY45jvg8hj21l8f9BHbznCXYz5hxdvkdhPFvh3fOg49-HkA_KLFFRhR0HxW87BTWmdIFWF8WdR8zATK4Xr0g=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIoWbn5cmxjpKadbHi_ZIiCMPDo0jVNLzv87UX2SVj743OddLj3kDEiWuEnJAnP2AllUEDhLSTufmF7Wl8Vt4sBLvLqUhl2aRy3fyPY2J_Q25TPrUO5_efinAwBWFIQkmJRh9Zq7f1fYaAuinGlLfbNJqFB2KxoOD2foGkJnGlXBze5mvkYxTQebEK9uV1nL2tVpMCsxHVMaOfsD4W0TIGcT1C2LzlyVqWSuOlCxWFDf8BxLnSMysFig_bFUWpHbuglY9juzgNBQFA4xWi7B-zMfZmxBUheKTVxPm-tTQBJTjE-ckk1tPTwUE4MRjhUFSgEca_xtOmmJKrz1bXxN-MUMgA2_9WyWrqV2RKBaJqiVjvCnTqYM6DLJQU9qap92XXHIvnNOtr7ZbSPqZeMyZSVBcUUOTC5kkbrjtRtffOg-dYk8TXhbkx3zCOW-zEYNOpnO_uO408209XiNxcBcpfAFcMD6g2js0lWCZJwkxokn8FyoHbCq1uJud06fGYhPROkzlRZfwh4Bcu9dHDh2s4GP47TPlyr2jHZqDPeSEhj6q5ASP8ZvTmVFfl0ZRfEQ0woeKMyWI4O_UAx078DbMZoI-LOXVVG9OBQ8FKAFRxg-DRqRB2QstVHGS0fBAXiKakuaoPNiSjtEligW7q5CtqSvT55LyeCnTlfQIbKSB-ZuSN7rj-rbc99KjJ01rykM1Zpgr-D-76cteXFtw8V9SSaym5vUHiKkaCCWyw=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIoCT8-zO4sjgfUtGKSSAqugLLfcy6IzhpgsLqwSaQoD52Nc903uv5ZMkD5H3pHxvyzQxMgKGLMulQmq0AqBCgY4WnqyONvGNjiQJcznheusdXuG2XxxZ3GpnA05KdbXBCzSlM9CQ3MUIbh0PiEfjAOqsGoigQOylhojjoO1EmyOri8ftM9GxfE-h1DW66PLMkpPF9bxpB31LZbawgrDvGH3a1Kbi9r-Zn9lYoA7k3Hp0eQJmNSDDYLXCNEGXcmZAdJcIx9gsVnpL9C_vNHjHU1xOpiTxduY1HfOTbuhDL0ikvJPzaWntUOvOxPOYFrdhnw7QO2PuN-EEHQH3uRIzXq1cj5R3LWl9ru-ycsZjycOQ91kMqBb5foy8SKSPX0fBoupB1jHhfuSL7Fq9__-RV8L9ZuwwILg0gKllxt51Hz7wFESej70NW1yCtzCchBOVKqXlbSLI3knhVgWtgZVwMvjNXtE3o0otyOO_5qABIhIpK7u1qtH3_CxsCSVLmA4SrqOM2c3gq_qqUTbTdbsGt7Ryi7eRnj6o3HHjnUc7gLC9U3JYItkJ4IqFagirhtZdfc6cyyj0CoZr8F1FERT9K58GTljdxefBWazdY0_J9VNjtg14RwkPbQqm5pKxmxbR7msUJXoF7gzenJu9pqKdauV0ddBSO6T3B_-ZK_SFtHHamfNN5s4wu7XZegONfCKI-qg5wJWa1hKkkvJQ43kWAxv36T3ODjInGX2YA=s1396-w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqdGbQ23li_rM2tpksSgGj2SfMyaLckd5xvj0T9ItfZ7RJMa4IR283cB64Uxux1tk2W3lw0LUdiPRdo_4oRxuTR7e5nyx9IrbgvZ5f0TgElOvn9zYMa9IvhVpsBUIzdgiEFsD93NG2GVnodxZ_UJY7ax28O6yBHn__cMcPRcVMfI_tZdmNWlMlADLem3yDxjmoAVoPl0TFC11gUU6j02isXIu1AV4A-y0av6mmjzQcwajtnQUgBVFxvaBFGrbbA2Qgpov8BiQhOm-utT8ZCrji4_sU3ceNADzqpcwUnahk68-Wqlz0FHnrJojZ7L6RAEB7FPAxSpYrkOOLTJSl2jy-3Ha7kj_JzoYG347FMn0hUvsTAn2igbmq_EY-tBVeqG89y921bJ0rN1BSGOhDC_BRWosNN5zrEkKcIasacSKQxDTXozXgG57oY4L-ANBNR4ZsnLXuTpGuVzDiPlUVsCec3HRzTVjmt0vE2zrDaNDGQcR1C0TKlNKDsI4kiW44YbXBJPwH3y6xVBY_OfxKZ3z8Y1wTHlQTfMvidPmLmO5NqzY36NjH98OJCd3U6yWz6HVQ-BXcXvIau4ZNg_vIhq2IgRQnG_RavJR5FJrBkCqXR1NSR751Iuv9oVVvNGHhn0pcV2jMRgeXoX-rTApj_OP09w8PlTTCVmHFOQJMNLXt6thaZrze1zDLHK9sjCTvyQGe2iIdiFVgYyMZVYrENGwFFug52t4_y1LPQtg=s1396-w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqrRhrZLXYdbk7IvuLWEDgwEELyj9JSUdgyd03LrTDacGtpwVNvruvhVPLo7L8Afe7nyUs670aY6Z1FsHgj9lEwcQSdRRS61Da9j6pBcEeK0sWnDUE4jEIi992uKYoQd3j2lhaDIDg_HfgvgyGx1QVUMKX67kONmJcSt1R3fvEeYvwdmNouqxFuEnjOA2DJgdH6Jg30OuiJpvkw52WEoiGXRkOkze60LdxOLxT7NWgP3ePbU-As8GTU9ERTmpUjwP3NujYOehcgn8GmqGrD8Tw6xZlSXXRYFRljOauAOhVa32Nz-KMjm9djRToQghczVU2Lgyp0MUKjLOGmoXCYehY9URbI55wVx4QkfGNKsLPhF7ALzt_AOD6-SLXoLi7qwMwPGkQLKxdSMyWmzneYTKqeFRyBICOmh9VHHmgUprYa_l3T5sr3g6qNy7RZd92Lq0_DT9tKsCHuoA8_ia59iVdfYyrrRB3EzpQyOy-mPrCVxN1q0xP7yd3VhLSs2L1GyTd86tQgs8SleoOy1uwh68mVFduSrwXsLnOIYMPSuLHb5V2NleXoI7vBJYd3_7z0vIiNKoLZsjlGyJ34acoGHq1MsemVJSbp2W6bOx-tnUzQPnV4q46xpDXssodiY0gjXHTa6XBOMwxj_PgZc7meuJOjdIRE2atLRPzc0jeYhC72RjYNzmEsLh_pucVOVHohpmawc1nsANt-KR_efxCTMt20aVPSkRSvJspafw=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIqt6ci5YD1B8t1aEAGLQ51W8kcesSk-CT21OrGkVXkP_lsqX7fMY-1fPiHiIWx2E13H480eAGxxC49cT9fHfASFa5JnGVa2EmDK-la1S9Y8GJFiBnYMo5jrcTc_ymT_SCvjvNnrN_tzrMgpZDHTjcJRZ8YG7avht3XZAoAFbCakEAATTTBG6tRnHIXE4XOKRqCP7bpK9xMciYSTOshiuGB6ZpuJkMhd3PxoROcZawq3LLVzywFNrs7q7H_Qwa6vUVGg9E7SbEAgsX5EqwLbw-lqVTOupYH2dU0p3Ma6tO62IkKk2iwaLLHEmmkwWUPIfAFABOlFH8JqEIAmselCG_mFqkc1fgNN7D7YA_gXgzVTNvhJzCFgaHVeiALZi8Ltdta5lfPrC16oIFjyNXyfarhGYBhUEIiIcla0uoA7GC_NNqUPu7dKZsGnC56q9EjDOxOZ0drFPOPIrGtTtBJJDz_Pi81lkdByjABKKiIIixrXfX6xdRpGl0MoqBWO0TAqO_eH5-47Ph0oGuo9uIvP11U6TH2EzaFN-1AcBYPYuvdNYOg7AU8nqACNu3KepWFeFlFjilQDgzLg-6xWfGdgzWIevPJvO7x8FCCQpUObmMs0Yrtu-WgLasfB61mIlDDFELL-sAMZIew0eXj7-Eb12vcfPSjy0fWmz5quvkj-z_8wGLsf7hKj42bj6nN79fXHKxteSPrIoRvZP1XEYX1eEMgiTHHUtZgkF7BReQ=s1274-w1274-h588-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIrTmHGvw9UhQeitGWS0c77QCxV4fp1LuOTCoXB5nrjKVxgqRqpZqfT-kdHHqdr8plDTEECOJfta7UrKtgI96WhxwijuiYpMBvVji1iylh4EG062shW6cbwievXpLz8hjB_pPMAzp7D9wnck8lOw9sC3JdMbFSnKDNw4aRPit6IPjj5dLnJQlty8TXjuyNRgxeogQGJWs2kbxE5g_T4_09qBsvootkaTfhBvhl3H3H64sG5H0UV1aJGXYNIsQesuKkUG7acmZ-KKVALCNXlCR6XYNBdUXaNhIDFaIsVod2VVGpyArHPCAdoFSNbUxnmh8NRJzoze3uWchpspxwvO2VnW9_OQb7q4dI4zSexkAeLIO-b4_FBDyz2Ush8EMlhNp5RC0mbL8TOedE-V7eQuUz6I8nru49PCRpFwJGRkO2xxQEfitk3hsFPcwnnQ63IVtugvaTQ5norMU5SFt_Jv6-3to8WsR6UJaUrJAWUuOyICaEyGELb_XOwN2L62pPkIfXuEM-WVw-2CCfDzlKtdnNwvG1U4pZeGx2YocByN10k_L79ctHuc7NsPm2v9vgYm93aD7wcO9jRa5hvFRuKKR-JNxW3roFYppV2WF9EK9-_btwlsfkpLD000q1GnzR8qI93K8IzcoQRR872LWAcOoVkrKlZ2zSKMaAeR37eExuzCs1C5BwWi6_9AuTsuN0eLQqayDMQlnLZOxi-RGa3WqNMIEyOMmKRaZ9eq7A=s1396-w1048-h1396-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIot38NM2RsEQzOM--3hkKK4Nm4aeQ3Xb-w9nhjAh77DHJEz3GAs4mGaX-tVkkmXXuqYp6U-nDpyyk4GJEbSscMxb3dh0KDaKwmVFG2q9_xXZh7wGgJ83MqV41AYPMm-YFKCH3nDeX0WD6ZqzH6IodOFSDnwOwGFSQnPDeOa7xMs6tO9m26K5LLudQvB8r5EDPNAlTn3nQUFWM0VxuUV5AtqSAJ-G3myNcbOGLDWyXvky3WhSp621rf7ImhuwsX3yWY9xNwH6uiKDmT_7miZrPYVHsTrLLV_tqpjjgmXWQ8I5EexvKSy47zy-dHr_Iqyi-on03mb9dRzt5AWYYudFGUWD_YL5emtrz06zsZhR0RyQ6sFU-uGyatcO-60XVIxnUeInESYFoVuPc8rgODzutEBf2DOihe8dBTm4nyXjzu-56A4Pm9owqaXkDDZbputbrlQvJItOv7izT4Tu7Aa42_QHHzYy4n9n86rEVj6joMt46vERFwDnGDBSmj53b0W5F9UkjkpfCoRsKQIM-t46BiFSlES5SSAZ6w_XJXAHIauBtYWlIJ4ULwenuVrV0hax02kQiUiFNDo9WTtrVRsR79jEMM6QQwbGI-fSmm5_gjtvSMduynHi1_VF1Gho5q6K4bjAeNKK2YSBCE6VkYxBlR4Y7ivy_TNeAu-DeInzkBiBujskCmEY0fPu3GmVfmgABUqoHsr-b97F7OM2KWdnjL5RITxUKTIFOm0PQ=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIpH4Li_-g0cQXRO6PcWcyFRztr3Mii0QTe2fqBUai-Cx5JfoACTlutaDzDc32XiGoy1OMTwXngoEkqSKnl6Dj7EWJ9AhXiwlrgZKSLjHm5PUFOqvjprSqsKn-C2ATE6D-uOECalcGXfS9OfozySFRau9p2gn97-cejlgLuHpIEWRdt46JwD_ikWRh1GtVP5A_XC_YaZjkC2nhlfsIsLOTgTmH9JBlLUWfwV5sFWdYU9NR_Qp95gniIk20zrlQtlKenJZhtaoBeh-BiSyMxGp-v6yVyhNXkHGp3oNH-sWfqiWBbf-5LZfPR0ARdee_zPP89_XPu2Exl-bvHIPZ8cRORB9Rr5oTW-ior9vcFxOmZdRbcIJwJV0uzXoqmnYvfHWFoGTXbR6zhMGfst1eY7Uj8S-2OFDN5HGi94PWAN1ElVuP4Avc8LgHlbUHtI3quTv6u4yr8GbN7UqyiEW77x5kTGK6-1goDFdpfL4KNZ74wAFzhpqarQZMQ6XnatJc9NS-AlMdsHvxiP9s49FJ61QPOcnNKmvH_lZesY798YdFKEsx0uYBI8INKyQFAlhEDa3_szfnONlOduSKDKjIftwuSa7crdfz5l0pzcJ9SkUl-XXJnh9suwifxc6i3l_QQr6474saEmcKmhlwYbbESZ9sbOhF8t_JsrG4Jc4LsQVUTMNEi-JCVzUiA5iQtiWp3WLs_212WVo8N4jIqNqVpqSq8TUP6oCqLpD3Uj8Q=s1274-w1274-h956-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/fife/ABSRlIpelaWhgNGmi8HK4Ct7nXeir_LwwM6pXfQ_d2QTgyCXLn0DOeuL0_umCnI97bXD_vkedRKeSlvIWN2JxXk-aahwv6pLLiZrrpAw70y4YZfYVxpC6mB23r40vspargUvah_x9KSw1ZPsbZ52nt6i8Sq8A_uEFt82fhhfjX6_QvRGu5SHxQ_oF2HJJA_RONPnv1guQo7hYjHAmp2-Pay8Pu-Fs_CYp95PfjljD3wjQhPqc_MV28DQ-ILj3PpzAbB6hHxlD-3VkpPUNMb3PmOfB8CLXQ18ZvnuI-Wx_EA4VgIhUrfh5CrqXkK23hmAR2J2nGQDzqD5bQI8SaMQDvZ_Z9sXAPbkLz60WNlcC4YNeWwtn-wv-zzkR5iwNnA9ztOblS9nWEKnTIt0AELI4yNzXJ6PJxhcSKA1rbFE_5xcOaWx_Dk01qBBO1yaqDDi6Wk8tLJS8Qn39eaH_z9yLR1hG1gwM2XUwdV3iFobUCDeowPvLPY4peGMItevURPUyTm6MCfB5zr6V1nvHcHT2W0_R_77rL9Ajjh3PC2XnxN4E00TfUjfyG0KNoZp7K7oYWlLBnv9YeiKXYSRcv-mazh7jwsqJ2tPvIG4WV_fj-ppvDiSRiGU6wXZOdxcOY9mcC14pqeTmuz_6mCp7elq6epaVKFtvAkGXBeqb1qMWxl8TjStlpACYyuXLHPljC5Cd3jCpGIyqQ_2Rtjef6S5H1Bb4qPOuKfFduR31N8BOw=s1274-w1274-h718-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/bsTg7nmZsIzd03ezFlbrEw03g4qoDK2lucM6IsQBwl1qpQaOlYFG1hOf1ymL5dmYS22RClnXzJTWmtQ89muNT7zSHmOxxUVZeIzkFmPSRB_TrLPFKR6WLwUlzBE2BpYcalcl0NZsVQpBO1hDjhGLmjExCfy9pQPfQgWX2hJQAuXFsB6m-m2Teb4e2KymYvU3v_twxw8dlhS0Ls1ShIo8YP8oLbwGEv5lpd4-RalbXnRiDe_Wr87gAOKLpDnt5vi4vj3tOxDTcF6Hs2l6qL1EoLRkhumlk6pYEiSRrRAvzDt14sGqdz0bf-3cxCM0QFPFqeAkz47aS77jtGzrPT-A6clOP70fc7tLnpoSPCquLV00pcVgSqNbkpxVBHsG2O1SgO9Qat0Yx7ZYpRlzbkLnzeyakwjNWotvtwxUkes-BPXZIDzFydA-ynfpaaV3Q6OFw3EByKqaEUi01og2JlIm9EwLXdSxi6is_mZjNBYvic7RjX8ZHpqqdp1TMMCU42Js-fde76tUqMAcPg-lvj_zEZueQcMRKc1NiUS65LTmsTZkv6VymViEtdq7_XHdw6OoDjEWv5aiPLJlNUSrU2MmqBk0J5lV00H9X9u5EYjWQJMTZf-WNzBsGw2aY6Xzdv9SBbt5qtIgxydT4oVfAWXhRNmGgT1mUVQryoRduo84LMDIEf-iAmiqm-fRgZbzgQ=w744-h558-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/BijFhPygA9j0fkK7qA5MFQIfum-tGnK-x4oTq66WyewLSc2yJLTfDsur6yOZ1CtrhhO4b9cBykA64ddfDsbakcCCzyCYgTTIYJfRO5Tg11XBrRDLd-32hTrHs5z8o8Y-IvJGJAskvLscAYE66Ts5w8maKV5UNaUPsssZQXrU29J8xRZmDAoehFbdj9xvdynIUAEIgKiHm0pPJNXQvE_5j61hBiwkQBwFjSyYBSr_z9ozkH1UaGPbFqM3MQloGySI-91mjpUo7Yt2aUHmx66EiMHIGjG1xF8IEMsZy3vhRk_W0qyV0XfCV9Oq2hS_YYkGQAaJIOC9RCsenl-xQWqoDxSfhXkpMfHuTrJ6lHoaReZH9e0zWWh6G9jgSZvCIN5xjSnnmUC_Zs65VnBkwrzbao7BDSGadehpA2fbmHKicExrYZ1WxIlihUd6ST8eGw8BORptSDhhVb-i75JPLmmdDM994dtt3dmw-3xcFiul_qx2OPs2uNH7AXdA9AlvkC7H_UO3Ju_0p28f22r7tuiNBMo-5ugM9SzEDGw98e-7a-9oCeau0e0cCyiNw-bHrxht_VYqvm-3Cainh0E7NdEQijhy7JNVuXmP2VbAbG1_G8t-A6gycE7JpGs_Pw1uQpV5jvfWaSnCNq528VsD9ogt8VirbgLPghik1D5h7LUVW-LIApGf8I4HZEZBZv3QFw=w1464-h1098-no?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/n6jfU7FMoJs1konKMoRsTPuRbneVs6WNlF1AtJ5JpN5vEXZdkB24eFmCjg4vyQwJ2F3K-zWHLr97ECj0U7LU1dRedCKOygVUV0JSeQBajKMMVS8Tfu-VwaVQK-AYQr47XJGUd-U5mb8=w2400</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/46ULbuQXBxmHzss6qhp9ojBjR2ka9UnUmqflWHRc3z6bYWYLrAncwlYnTe7pYwjRd3QZkSVI8s_X55Fhbiu1ZZZyZWZfWhgrJgGJvDC91S5RrGKcq0wDv3cQ6K27XiY3ySpZwsaSiFo=w2400</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/hRQsvLqY2jdeD4tZdDC93J7nj-6yncMLZqUOBEWVYCfK3HUGyDYh-XoXLa-JzCwy9-y5EdRvueptWM3CH0JFO5d3smcCphhxcgxmcLMGsVxg5cw0d1K45kSShMDeCDVfyGbQSNYOW48=w2400</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/A4zBD3WhaHM5f2cPZZjC_l4qdNR7WjzjulWwyFgwVQ1f7ccmPvB_RRbKQQ8qTP0U1drkZKESc6hAK5eBAMPZcvzrJ0mjr1xz5msQPogxCNv9RO4mB3cJC9z6II4_wtPV0OBJuVSW6dM=w2400</t>
   </si>
 </sst>
 </file>
@@ -1097,14 +1104,14 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1118,7 +1125,7 @@
         <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1129,10 +1136,10 @@
         <v>44180</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1143,10 +1150,10 @@
         <v>44180</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1160,35 +1167,35 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <v>44178</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1">
         <v>44168</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1199,24 +1206,24 @@
         <v>44161</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>44154</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1227,10 +1234,10 @@
         <v>44148</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1241,10 +1248,10 @@
         <v>44148</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1255,24 +1262,24 @@
         <v>44134</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>44120</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1283,10 +1290,10 @@
         <v>44101</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1300,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1311,10 +1318,10 @@
         <v>44087</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1325,10 +1332,10 @@
         <v>44079</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1339,10 +1346,10 @@
         <v>44073</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1353,10 +1360,10 @@
         <v>44069</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1367,10 +1374,10 @@
         <v>44057</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1381,7 +1388,7 @@
         <v>44035</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -1395,10 +1402,10 @@
         <v>44011</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1409,10 +1416,10 @@
         <v>44010</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1423,10 +1430,10 @@
         <v>44009</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1437,24 +1444,24 @@
         <v>44009</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1">
         <v>43982</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1465,4 +1472,29 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D040420A-BDEB-6643-AB92-E71B41E54394}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>